<commit_message>
Actualizacion del plan de proyecto, integracion de hitos actualizados y personal nuevo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
+++ b/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,30 +19,30 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" name="Complej." vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_4" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Complej." vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="Complej." vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_2" vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_4" vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_Toc120446010" vbProcedure="false">Presentación!$A$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_Toc120446011" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_Toc120446011" vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Presentación"</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_Toc120446010" vbProcedure="false">'Datos Generales'!$A$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_Toc120446011" vbProcedure="false">'Datos Generales'!$A$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Sheet_Title" vbProcedure="false">"Datos Generales"</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_Toc109545561" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_Toc109545561" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_Toc120446019" vbProcedure="false">'Recursos Humanos'!$A$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Sheet_Title" vbProcedure="false">"Recursos Humanos"</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Sheet_Title" vbProcedure="false">"Capacitaciones"</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="Complej." vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="Complej." vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Sheet_Title" vbProcedure="false">"Plan Comunicación"</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Sheet_Title" vbProcedure="false">"Recursos Materiales"</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="Complej." vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
@@ -51,14 +51,10 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Sheet_Title" vbProcedure="false">"Plan Riesgos"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -888,7 +884,7 @@
     <numFmt numFmtId="172" formatCode="MMM\-YY"/>
     <numFmt numFmtId="173" formatCode="0%"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1043,13 +1039,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1386,15 +1375,15 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="173" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="173" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="154">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1475,6 +1464,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1484,10 +1477,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1696,10 +1685,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1719,11 +1704,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1735,7 +1720,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1759,11 +1744,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1791,7 +1776,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1827,11 +1812,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="28" fillId="7" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="173" fontId="27" fillId="7" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="7" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="7" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1843,11 +1828,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1955,7 +1940,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="28" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="27" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1971,11 +1956,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1987,23 +1972,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2213,8 +2198,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4411,144 +4396,146 @@
       <c r="C15" s="19" t="n">
         <v>42380</v>
       </c>
-      <c r="D15" s="19" t="n">
+      <c r="D15" s="20" t="n">
         <v>42380</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="21" t="n">
+      <c r="C16" s="22" t="n">
         <v>42402</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="20" t="n">
+        <v>42402</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="21" t="n">
+      <c r="C17" s="22" t="n">
         <v>42432</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="21" t="n">
+      <c r="C18" s="22" t="n">
         <v>42463</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="21" t="n">
+      <c r="C19" s="22" t="n">
         <v>42493</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="21" t="n">
+      <c r="C20" s="22" t="n">
         <v>42524</v>
       </c>
-      <c r="D20" s="21"/>
+      <c r="D20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="21" t="n">
+      <c r="C21" s="22" t="n">
         <v>42554</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="21" t="n">
+      <c r="C22" s="22" t="n">
         <v>42585</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="21" t="n">
+      <c r="C23" s="22" t="n">
         <v>42616</v>
       </c>
-      <c r="D23" s="21"/>
+      <c r="D23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="21" t="n">
+      <c r="C24" s="22" t="n">
         <v>42646</v>
       </c>
-      <c r="D24" s="21"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="21" t="n">
+      <c r="C25" s="22" t="n">
         <v>42677</v>
       </c>
-      <c r="D25" s="21"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="21" t="n">
+      <c r="C26" s="22" t="n">
         <v>42707</v>
       </c>
-      <c r="D26" s="21"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -4661,6 +4648,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="10" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5216,7 +5204,7 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5479,88 +5467,88 @@
       <c r="A2" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="75" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="77" t="n">
+      <c r="D2" s="76" t="n">
         <v>42380</v>
       </c>
-      <c r="E2" s="77" t="n">
+      <c r="E2" s="76" t="n">
         <v>42380</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="78"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="78"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="78"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="78"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="78"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6664,13 +6652,13 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="79" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -7692,19 +7680,19 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="80" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="80" t="s">
         <v>152</v>
       </c>
       <c r="F3" s="0"/>
@@ -8728,19 +8716,19 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="81" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="82" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="84" t="s">
+      <c r="E4" s="83" t="s">
         <v>156</v>
       </c>
       <c r="F4" s="0"/>
@@ -9763,67 +9751,67 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="87" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="85" t="s">
+    <row r="5" s="86" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="85" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" s="87" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="85" t="s">
+    <row r="6" s="86" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="85" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" s="87" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="85"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="86"/>
-    </row>
-    <row r="8" s="87" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="85"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="86"/>
+    <row r="7" s="86" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="85"/>
+    </row>
+    <row r="8" s="86" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="85"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9886,175 +9874,175 @@
       <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="87" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="87" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="87" t="s">
         <v>168</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="87" t="s">
         <v>169</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="87" t="s">
         <v>170</v>
       </c>
       <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="88" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="D4" s="91" t="n">
+      <c r="D4" s="90" t="n">
         <v>42380</v>
       </c>
-      <c r="E4" s="91" t="n">
+      <c r="E4" s="90" t="n">
         <v>42373</v>
       </c>
-      <c r="F4" s="90"/>
-      <c r="I4" s="92"/>
+      <c r="F4" s="89"/>
+      <c r="I4" s="91"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="D5" s="91" t="n">
+      <c r="D5" s="90" t="n">
         <v>42380</v>
       </c>
-      <c r="E5" s="91" t="n">
+      <c r="E5" s="90" t="n">
         <v>42373</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="I5" s="92"/>
+      <c r="F5" s="89"/>
+      <c r="I5" s="91"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="88" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="89" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="89" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="91" t="n">
+      <c r="D6" s="90" t="n">
         <v>42380</v>
       </c>
-      <c r="E6" s="91" t="n">
+      <c r="E6" s="90" t="n">
         <v>42373</v>
       </c>
-      <c r="F6" s="90"/>
-      <c r="I6" s="92"/>
+      <c r="F6" s="89"/>
+      <c r="I6" s="91"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="91" t="n">
+      <c r="D7" s="90" t="n">
         <v>42380</v>
       </c>
-      <c r="E7" s="91" t="n">
+      <c r="E7" s="90" t="n">
         <v>42373</v>
       </c>
-      <c r="F7" s="90"/>
-      <c r="I7" s="92"/>
+      <c r="F7" s="89"/>
+      <c r="I7" s="91"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="88" t="s">
         <v>179</v>
       </c>
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="91" t="n">
+      <c r="D8" s="90" t="n">
         <v>42380</v>
       </c>
-      <c r="E8" s="91" t="n">
+      <c r="E8" s="90" t="n">
         <v>42373</v>
       </c>
-      <c r="F8" s="90"/>
+      <c r="F8" s="89"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="93"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="90"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="89"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="89"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="90"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="89"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="90"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="89"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="89"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="90"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="89"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="90"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="90"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="90"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
+      <c r="A15" s="89"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10078,7 +10066,7 @@
   </sheetPr>
   <dimension ref="A1:JA33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -10099,10 +10087,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="96"/>
+      <c r="A1" s="95"/>
       <c r="B1" s="0"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -10143,19 +10131,19 @@
       <c r="JA1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
@@ -10177,31 +10165,31 @@
       <c r="AD2" s="0"/>
       <c r="AE2" s="0"/>
       <c r="AF2" s="0"/>
-      <c r="IR2" s="99" t="s">
+      <c r="IR2" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="IS2" s="99"/>
-      <c r="IT2" s="99"/>
-      <c r="IU2" s="99"/>
-      <c r="IV2" s="99"/>
-      <c r="IW2" s="99"/>
-      <c r="IX2" s="99"/>
-      <c r="IY2" s="99"/>
-      <c r="IZ2" s="99"/>
-      <c r="JA2" s="99"/>
+      <c r="IS2" s="98"/>
+      <c r="IT2" s="98"/>
+      <c r="IU2" s="98"/>
+      <c r="IV2" s="98"/>
+      <c r="IW2" s="98"/>
+      <c r="IX2" s="98"/>
+      <c r="IY2" s="98"/>
+      <c r="IZ2" s="98"/>
+      <c r="JA2" s="98"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
+      <c r="A3" s="97"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
@@ -10221,10 +10209,10 @@
       <c r="AB3" s="0"/>
       <c r="AC3" s="0"/>
       <c r="AD3" s="0"/>
-      <c r="AE3" s="100" t="s">
+      <c r="AE3" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="AF3" s="100" t="s">
+      <c r="AF3" s="99" t="s">
         <v>183</v>
       </c>
       <c r="IS3" s="0"/>
@@ -10237,37 +10225,37 @@
       <c r="IZ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="101" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="102" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="G4" s="103" t="s">
+      <c r="G4" s="102" t="s">
         <v>190</v>
       </c>
-      <c r="H4" s="103" t="s">
+      <c r="H4" s="102" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="103" t="s">
+      <c r="I4" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="J4" s="104" t="s">
+      <c r="J4" s="103" t="s">
         <v>193</v>
       </c>
-      <c r="K4" s="103" t="s">
+      <c r="K4" s="102" t="s">
         <v>194</v>
       </c>
       <c r="L4" s="0"/>
@@ -10289,10 +10277,10 @@
       <c r="AB4" s="0"/>
       <c r="AC4" s="0"/>
       <c r="AD4" s="0"/>
-      <c r="AE4" s="105" t="s">
+      <c r="AE4" s="104" t="s">
         <v>182</v>
       </c>
-      <c r="AF4" s="105" t="s">
+      <c r="AF4" s="104" t="s">
         <v>183</v>
       </c>
       <c r="IS4" s="0"/>
@@ -10305,38 +10293,38 @@
       <c r="IZ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="106" t="n">
+      <c r="A5" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="106" t="n">
+      <c r="C5" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="108" t="n">
+      <c r="D5" s="107" t="n">
         <v>0.6</v>
       </c>
-      <c r="E5" s="106" t="n">
+      <c r="E5" s="105" t="n">
         <f aca="false">PRODUCT(A5:D5)</f>
         <v>0.6</v>
       </c>
-      <c r="F5" s="106" t="n">
+      <c r="F5" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="G5" s="106" t="s">
         <v>196</v>
       </c>
-      <c r="H5" s="107" t="s">
+      <c r="H5" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="I5" s="109" t="s">
+      <c r="I5" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="J5" s="110" t="s">
+      <c r="J5" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="K5" s="111" t="s">
+      <c r="K5" s="110" t="s">
         <v>200</v>
       </c>
       <c r="L5" s="0"/>
@@ -10360,69 +10348,69 @@
       <c r="AD5" s="0"/>
       <c r="AE5" s="0"/>
       <c r="AF5" s="0"/>
-      <c r="IS5" s="112" t="s">
+      <c r="IS5" s="111" t="s">
         <v>201</v>
       </c>
-      <c r="IT5" s="113" t="s">
+      <c r="IT5" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="IU5" s="114" t="n">
+      <c r="IU5" s="113" t="n">
         <v>0.9</v>
       </c>
-      <c r="IV5" s="115" t="n">
+      <c r="IV5" s="114" t="n">
         <f aca="false">(IV10*IU5)</f>
         <v>0.9</v>
       </c>
-      <c r="IW5" s="116" t="n">
+      <c r="IW5" s="115" t="n">
         <f aca="false">(IW10*IU5)</f>
         <v>1.8</v>
       </c>
-      <c r="IX5" s="117" t="n">
+      <c r="IX5" s="116" t="n">
         <f aca="false">(IX10*IU5)</f>
         <v>2.7</v>
       </c>
-      <c r="IY5" s="118" t="n">
+      <c r="IY5" s="117" t="n">
         <f aca="false">(IY10*IU5)</f>
         <v>3.6</v>
       </c>
-      <c r="IZ5" s="119" t="n">
+      <c r="IZ5" s="118" t="n">
         <f aca="false">(IZ10*IU5)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="106" t="n">
+      <c r="A6" s="105" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="106" t="s">
         <v>203</v>
       </c>
-      <c r="C6" s="106" t="n">
+      <c r="C6" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="108" t="n">
+      <c r="D6" s="107" t="n">
         <v>0.2</v>
       </c>
-      <c r="E6" s="106" t="n">
+      <c r="E6" s="105" t="n">
         <f aca="false">PRODUCT(C6:D6)</f>
         <v>0.8</v>
       </c>
-      <c r="F6" s="106" t="n">
+      <c r="F6" s="105" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="107" t="s">
+      <c r="G6" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="111" t="s">
+      <c r="H6" s="110" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="109" t="s">
+      <c r="I6" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="J6" s="110" t="s">
+      <c r="J6" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="K6" s="111" t="s">
+      <c r="K6" s="110" t="s">
         <v>200</v>
       </c>
       <c r="L6" s="0"/>
@@ -10446,67 +10434,67 @@
       <c r="AD6" s="0"/>
       <c r="AE6" s="0"/>
       <c r="AF6" s="0"/>
-      <c r="IS6" s="112"/>
-      <c r="IT6" s="113" t="s">
+      <c r="IS6" s="111"/>
+      <c r="IT6" s="112" t="s">
         <v>206</v>
       </c>
-      <c r="IU6" s="114" t="n">
+      <c r="IU6" s="113" t="n">
         <v>0.7</v>
       </c>
-      <c r="IV6" s="120" t="n">
+      <c r="IV6" s="119" t="n">
         <f aca="false">(IV10*IU6)</f>
         <v>0.7</v>
       </c>
-      <c r="IW6" s="121" t="n">
+      <c r="IW6" s="120" t="n">
         <f aca="false">(IW10*IU6)</f>
         <v>1.4</v>
       </c>
-      <c r="IX6" s="122" t="n">
+      <c r="IX6" s="121" t="n">
         <f aca="false">(IX10*IU6)</f>
         <v>2.1</v>
       </c>
-      <c r="IY6" s="123" t="n">
+      <c r="IY6" s="122" t="n">
         <f aca="false">(IY10*IU6)</f>
         <v>2.8</v>
       </c>
-      <c r="IZ6" s="124" t="n">
+      <c r="IZ6" s="123" t="n">
         <f aca="false">(IZ10*IU6)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="106" t="n">
+      <c r="A7" s="105" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="106" t="s">
         <v>207</v>
       </c>
-      <c r="C7" s="106" t="n">
+      <c r="C7" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="108" t="n">
+      <c r="D7" s="107" t="n">
         <v>0.2</v>
       </c>
-      <c r="E7" s="106" t="n">
+      <c r="E7" s="105" t="n">
         <f aca="false">PRODUCT(C7:D7)</f>
         <v>0.8</v>
       </c>
-      <c r="F7" s="106" t="n">
+      <c r="F7" s="105" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="107" t="s">
+      <c r="G7" s="106" t="s">
         <v>208</v>
       </c>
-      <c r="H7" s="107" t="s">
+      <c r="H7" s="106" t="s">
         <v>209</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="105" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="110" t="s">
+      <c r="J7" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="K7" s="111" t="s">
+      <c r="K7" s="110" t="s">
         <v>200</v>
       </c>
       <c r="L7" s="0"/>
@@ -10530,67 +10518,67 @@
       <c r="AD7" s="0"/>
       <c r="AE7" s="0"/>
       <c r="AF7" s="0"/>
-      <c r="IS7" s="112"/>
-      <c r="IT7" s="113" t="s">
+      <c r="IS7" s="111"/>
+      <c r="IT7" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="IU7" s="114" t="n">
+      <c r="IU7" s="113" t="n">
         <v>0.5</v>
       </c>
-      <c r="IV7" s="120" t="n">
+      <c r="IV7" s="119" t="n">
         <f aca="false">(IV10*IU7)</f>
         <v>0.5</v>
       </c>
-      <c r="IW7" s="125" t="n">
+      <c r="IW7" s="124" t="n">
         <f aca="false">(IW10*IU7)</f>
         <v>1</v>
       </c>
-      <c r="IX7" s="121" t="n">
+      <c r="IX7" s="120" t="n">
         <f aca="false">(IX10*IU7)</f>
         <v>1.5</v>
       </c>
-      <c r="IY7" s="121" t="n">
+      <c r="IY7" s="120" t="n">
         <f aca="false">(IY10*IU7)</f>
         <v>2</v>
       </c>
-      <c r="IZ7" s="126" t="n">
+      <c r="IZ7" s="125" t="n">
         <f aca="false">(IZ10*IU7)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="106" t="n">
+      <c r="A8" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="106" t="s">
         <v>211</v>
       </c>
-      <c r="C8" s="106" t="n">
+      <c r="C8" s="105" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="108" t="n">
+      <c r="D8" s="107" t="n">
         <v>0.01</v>
       </c>
-      <c r="E8" s="106" t="n">
+      <c r="E8" s="105" t="n">
         <f aca="false">PRODUCT(C8:D8)</f>
         <v>0.05</v>
       </c>
-      <c r="F8" s="106" t="n">
+      <c r="F8" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="G8" s="107" t="s">
+      <c r="G8" s="106" t="s">
         <v>212</v>
       </c>
-      <c r="H8" s="107" t="s">
+      <c r="H8" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="I8" s="106" t="s">
+      <c r="I8" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="110" t="s">
+      <c r="J8" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="K8" s="111" t="s">
+      <c r="K8" s="110" t="s">
         <v>200</v>
       </c>
       <c r="L8" s="0"/>
@@ -10614,67 +10602,67 @@
       <c r="AD8" s="0"/>
       <c r="AE8" s="0"/>
       <c r="AF8" s="0"/>
-      <c r="IS8" s="112"/>
-      <c r="IT8" s="113" t="s">
+      <c r="IS8" s="111"/>
+      <c r="IT8" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="IU8" s="114" t="n">
+      <c r="IU8" s="113" t="n">
         <v>0.3</v>
       </c>
-      <c r="IV8" s="127" t="n">
+      <c r="IV8" s="126" t="n">
         <f aca="false">(IV10*IU8)</f>
         <v>0.3</v>
       </c>
-      <c r="IW8" s="128" t="n">
+      <c r="IW8" s="127" t="n">
         <f aca="false">(IW10*IU8)</f>
         <v>0.6</v>
       </c>
-      <c r="IX8" s="121" t="n">
+      <c r="IX8" s="120" t="n">
         <f aca="false">(IX10*IU8)</f>
         <v>0.9</v>
       </c>
-      <c r="IY8" s="121" t="n">
+      <c r="IY8" s="120" t="n">
         <f aca="false">(IY10*IU8)</f>
         <v>1.2</v>
       </c>
-      <c r="IZ8" s="129" t="n">
+      <c r="IZ8" s="128" t="n">
         <f aca="false">(IZ10*IU8)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="106" t="n">
+      <c r="A9" s="105" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="106" t="s">
         <v>215</v>
       </c>
-      <c r="C9" s="106" t="n">
+      <c r="C9" s="105" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="108" t="n">
+      <c r="D9" s="107" t="n">
         <v>0.05</v>
       </c>
-      <c r="E9" s="106" t="n">
+      <c r="E9" s="105" t="n">
         <f aca="false">PRODUCT(C9:D9)</f>
         <v>0.25</v>
       </c>
-      <c r="F9" s="106" t="n">
+      <c r="F9" s="105" t="n">
         <v>4</v>
       </c>
-      <c r="G9" s="107" t="s">
+      <c r="G9" s="106" t="s">
         <v>216</v>
       </c>
-      <c r="H9" s="107" t="s">
+      <c r="H9" s="106" t="s">
         <v>217</v>
       </c>
-      <c r="I9" s="106" t="s">
+      <c r="I9" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="110" t="s">
+      <c r="J9" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="K9" s="111" t="s">
+      <c r="K9" s="110" t="s">
         <v>200</v>
       </c>
       <c r="L9" s="0"/>
@@ -10698,67 +10686,67 @@
       <c r="AD9" s="0"/>
       <c r="AE9" s="0"/>
       <c r="AF9" s="0"/>
-      <c r="IS9" s="112"/>
-      <c r="IT9" s="113" t="s">
+      <c r="IS9" s="111"/>
+      <c r="IT9" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="IU9" s="130" t="n">
+      <c r="IU9" s="129" t="n">
         <v>0.1</v>
       </c>
-      <c r="IV9" s="131" t="n">
+      <c r="IV9" s="130" t="n">
         <f aca="false">(IV10*IU9)</f>
         <v>0.1</v>
       </c>
-      <c r="IW9" s="132" t="n">
+      <c r="IW9" s="131" t="n">
         <f aca="false">(IW10*IU9)</f>
         <v>0.2</v>
       </c>
-      <c r="IX9" s="133" t="n">
+      <c r="IX9" s="132" t="n">
         <f aca="false">(IX10*IV9)</f>
         <v>0.3</v>
       </c>
-      <c r="IY9" s="133" t="n">
+      <c r="IY9" s="132" t="n">
         <f aca="false">(IY10*IU9)</f>
         <v>0.4</v>
       </c>
-      <c r="IZ9" s="134" t="n">
+      <c r="IZ9" s="133" t="n">
         <f aca="false">(IZ10*IU9)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="135" t="n">
+      <c r="A10" s="134" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="106" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="106" t="n">
+      <c r="C10" s="105" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="108" t="n">
+      <c r="D10" s="107" t="n">
         <v>0.2</v>
       </c>
-      <c r="E10" s="106" t="n">
+      <c r="E10" s="105" t="n">
         <f aca="false">PRODUCT(C10:D10)</f>
         <v>1</v>
       </c>
-      <c r="F10" s="106" t="n">
+      <c r="F10" s="105" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="107" t="s">
+      <c r="G10" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="107" t="s">
+      <c r="H10" s="106" t="s">
         <v>220</v>
       </c>
-      <c r="I10" s="106" t="s">
+      <c r="I10" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="110" t="s">
+      <c r="J10" s="109" t="s">
         <v>199</v>
       </c>
-      <c r="K10" s="111" t="s">
+      <c r="K10" s="110" t="s">
         <v>200</v>
       </c>
       <c r="L10" s="0"/>
@@ -10782,42 +10770,42 @@
       <c r="AD10" s="0"/>
       <c r="AE10" s="0"/>
       <c r="AF10" s="0"/>
-      <c r="IS10" s="136"/>
+      <c r="IS10" s="135"/>
       <c r="IT10" s="0"/>
-      <c r="IU10" s="113"/>
-      <c r="IV10" s="114" t="n">
+      <c r="IU10" s="112"/>
+      <c r="IV10" s="113" t="n">
         <v>1</v>
       </c>
-      <c r="IW10" s="114" t="n">
+      <c r="IW10" s="113" t="n">
         <v>2</v>
       </c>
-      <c r="IX10" s="114" t="n">
+      <c r="IX10" s="113" t="n">
         <v>3</v>
       </c>
-      <c r="IY10" s="114" t="n">
+      <c r="IY10" s="113" t="n">
         <v>4</v>
       </c>
-      <c r="IZ10" s="137" t="n">
+      <c r="IZ10" s="136" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="138" t="n">
+      <c r="A11" s="137" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="139"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="138" t="n">
+      <c r="B11" s="138"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="137" t="n">
         <f aca="false">PRODUCT(C11:D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="138"/>
-      <c r="G11" s="141"/>
-      <c r="H11" s="139"/>
-      <c r="I11" s="142"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="141"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="140"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
@@ -10839,42 +10827,42 @@
       <c r="AD11" s="0"/>
       <c r="AE11" s="0"/>
       <c r="AF11" s="0"/>
-      <c r="IS11" s="136"/>
+      <c r="IS11" s="135"/>
       <c r="IT11" s="0"/>
       <c r="IU11" s="0"/>
-      <c r="IV11" s="113" t="s">
+      <c r="IV11" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="IW11" s="113" t="s">
+      <c r="IW11" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="IX11" s="113" t="s">
+      <c r="IX11" s="112" t="s">
         <v>221</v>
       </c>
-      <c r="IY11" s="113" t="s">
+      <c r="IY11" s="112" t="s">
         <v>206</v>
       </c>
-      <c r="IZ11" s="144" t="s">
+      <c r="IZ11" s="143" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="138" t="n">
+      <c r="A12" s="137" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="138" t="n">
+      <c r="B12" s="138"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="137" t="n">
         <f aca="false">PRODUCT(C12:D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="138"/>
-      <c r="G12" s="141"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="142"/>
-      <c r="J12" s="143"/>
-      <c r="K12" s="141"/>
+      <c r="F12" s="137"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="140"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -10896,34 +10884,34 @@
       <c r="AD12" s="0"/>
       <c r="AE12" s="0"/>
       <c r="AF12" s="0"/>
-      <c r="IS12" s="136"/>
+      <c r="IS12" s="135"/>
       <c r="IT12" s="0"/>
-      <c r="IU12" s="114"/>
-      <c r="IV12" s="145" t="s">
+      <c r="IU12" s="113"/>
+      <c r="IV12" s="144" t="s">
         <v>222</v>
       </c>
-      <c r="IW12" s="145"/>
-      <c r="IX12" s="145"/>
-      <c r="IY12" s="145"/>
-      <c r="IZ12" s="145"/>
+      <c r="IW12" s="144"/>
+      <c r="IX12" s="144"/>
+      <c r="IY12" s="144"/>
+      <c r="IZ12" s="144"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="138" t="n">
+      <c r="A13" s="137" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="139"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="138" t="n">
+      <c r="B13" s="138"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="137" t="n">
         <f aca="false">PRODUCT(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="138"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="139"/>
-      <c r="I13" s="142"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="141"/>
+      <c r="F13" s="137"/>
+      <c r="G13" s="140"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="141"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="140"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -10945,32 +10933,32 @@
       <c r="AD13" s="0"/>
       <c r="AE13" s="0"/>
       <c r="AF13" s="0"/>
-      <c r="IS13" s="136"/>
+      <c r="IS13" s="135"/>
       <c r="IT13" s="0"/>
       <c r="IU13" s="0"/>
       <c r="IV13" s="0"/>
       <c r="IW13" s="0"/>
       <c r="IX13" s="0"/>
       <c r="IY13" s="0"/>
-      <c r="IZ13" s="146"/>
+      <c r="IZ13" s="145"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="138" t="n">
+      <c r="A14" s="137" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="139"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="140"/>
-      <c r="E14" s="138" t="n">
+      <c r="B14" s="138"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="139"/>
+      <c r="E14" s="137" t="n">
         <f aca="false">PRODUCT(C14:D14)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="138"/>
-      <c r="G14" s="141"/>
-      <c r="H14" s="139"/>
-      <c r="I14" s="142"/>
-      <c r="J14" s="143"/>
-      <c r="K14" s="141"/>
+      <c r="F14" s="137"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="141"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="140"/>
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
@@ -10992,22 +10980,22 @@
       <c r="AD14" s="0"/>
       <c r="AE14" s="0"/>
       <c r="AF14" s="0"/>
-      <c r="IS14" s="136"/>
+      <c r="IS14" s="135"/>
       <c r="IT14" s="0"/>
-      <c r="IU14" s="105"/>
-      <c r="IV14" s="105"/>
-      <c r="IW14" s="105"/>
-      <c r="IX14" s="105"/>
-      <c r="IY14" s="105"/>
-      <c r="IZ14" s="147"/>
+      <c r="IU14" s="104"/>
+      <c r="IV14" s="104"/>
+      <c r="IW14" s="104"/>
+      <c r="IX14" s="104"/>
+      <c r="IY14" s="104"/>
+      <c r="IZ14" s="146"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="148"/>
-      <c r="B15" s="148"/>
-      <c r="C15" s="148"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
+      <c r="A15" s="147"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="147"/>
+      <c r="F15" s="147"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
@@ -11036,12 +11024,12 @@
       <c r="AF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="148"/>
-      <c r="B16" s="148"/>
-      <c r="C16" s="148"/>
-      <c r="D16" s="148"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
+      <c r="A16" s="147"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="147"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="147"/>
+      <c r="F16" s="147"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -11070,12 +11058,12 @@
       <c r="AF16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="148"/>
-      <c r="B17" s="148"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="148"/>
-      <c r="F17" s="148"/>
+      <c r="A17" s="147"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="147"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="147"/>
+      <c r="F17" s="147"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -11104,14 +11092,14 @@
       <c r="AF17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="149" t="s">
+      <c r="A18" s="148" t="s">
         <v>223</v>
       </c>
-      <c r="B18" s="149"/>
-      <c r="C18" s="149"/>
-      <c r="D18" s="148"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
+      <c r="B18" s="148"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="147"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -11140,18 +11128,18 @@
       <c r="AF18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="149" t="s">
         <v>224</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="150" t="s">
         <v>225</v>
       </c>
-      <c r="C19" s="150" t="s">
+      <c r="C19" s="149" t="s">
         <v>226</v>
       </c>
-      <c r="D19" s="148"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
+      <c r="D19" s="147"/>
+      <c r="E19" s="147"/>
+      <c r="F19" s="147"/>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -11180,18 +11168,18 @@
       <c r="AF19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="150" t="n">
+      <c r="A20" s="149" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="149" t="s">
         <v>227</v>
       </c>
-      <c r="C20" s="150" t="s">
+      <c r="C20" s="149" t="s">
         <v>228</v>
       </c>
-      <c r="D20" s="152"/>
-      <c r="E20" s="152"/>
-      <c r="F20" s="148"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="147"/>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -11220,13 +11208,13 @@
       <c r="AF20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="153" t="n">
+      <c r="A21" s="152" t="n">
         <v>2</v>
       </c>
-      <c r="B21" s="153" t="s">
+      <c r="B21" s="152" t="s">
         <v>229</v>
       </c>
-      <c r="C21" s="153" t="s">
+      <c r="C21" s="152" t="s">
         <v>230</v>
       </c>
       <c r="D21" s="0"/>
@@ -11258,13 +11246,13 @@
       <c r="AF21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="153" t="n">
+      <c r="A22" s="152" t="n">
         <v>3</v>
       </c>
-      <c r="B22" s="153" t="s">
+      <c r="B22" s="152" t="s">
         <v>231</v>
       </c>
-      <c r="C22" s="153" t="s">
+      <c r="C22" s="152" t="s">
         <v>232</v>
       </c>
       <c r="D22" s="0"/>
@@ -11296,13 +11284,13 @@
       <c r="AF22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="153" t="n">
+      <c r="A23" s="152" t="n">
         <v>4</v>
       </c>
-      <c r="B23" s="153" t="s">
+      <c r="B23" s="152" t="s">
         <v>233</v>
       </c>
-      <c r="C23" s="153" t="s">
+      <c r="C23" s="152" t="s">
         <v>234</v>
       </c>
       <c r="D23" s="0"/>
@@ -11454,184 +11442,184 @@
       <c r="AF27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="148"/>
-      <c r="D28" s="148"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="96"/>
-      <c r="N28" s="96"/>
-      <c r="O28" s="96"/>
-      <c r="P28" s="96"/>
-      <c r="Q28" s="96"/>
-      <c r="R28" s="96"/>
-      <c r="S28" s="96"/>
-      <c r="T28" s="96"/>
-      <c r="U28" s="96"/>
-      <c r="V28" s="96"/>
-      <c r="W28" s="96"/>
-      <c r="X28" s="96"/>
-      <c r="Y28" s="96"/>
-      <c r="Z28" s="96"/>
-      <c r="AA28" s="96"/>
-      <c r="AB28" s="96"/>
-      <c r="AC28" s="96"/>
-      <c r="AD28" s="96"/>
-      <c r="AE28" s="96"/>
-      <c r="AF28" s="96"/>
+      <c r="C28" s="147"/>
+      <c r="D28" s="147"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="95"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="95"/>
+      <c r="M28" s="95"/>
+      <c r="N28" s="95"/>
+      <c r="O28" s="95"/>
+      <c r="P28" s="95"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="95"/>
+      <c r="S28" s="95"/>
+      <c r="T28" s="95"/>
+      <c r="U28" s="95"/>
+      <c r="V28" s="95"/>
+      <c r="W28" s="95"/>
+      <c r="X28" s="95"/>
+      <c r="Y28" s="95"/>
+      <c r="Z28" s="95"/>
+      <c r="AA28" s="95"/>
+      <c r="AB28" s="95"/>
+      <c r="AC28" s="95"/>
+      <c r="AD28" s="95"/>
+      <c r="AE28" s="95"/>
+      <c r="AF28" s="95"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="148"/>
-      <c r="D29" s="148"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="96"/>
-      <c r="I29" s="96"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
-      <c r="S29" s="96"/>
-      <c r="T29" s="96"/>
-      <c r="U29" s="96"/>
-      <c r="V29" s="96"/>
-      <c r="W29" s="96"/>
-      <c r="X29" s="96"/>
-      <c r="Y29" s="96"/>
-      <c r="Z29" s="96"/>
-      <c r="AA29" s="96"/>
-      <c r="AB29" s="96"/>
-      <c r="AC29" s="96"/>
-      <c r="AD29" s="96"/>
-      <c r="AE29" s="96"/>
-      <c r="AF29" s="96"/>
+      <c r="C29" s="147"/>
+      <c r="D29" s="147"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="95"/>
+      <c r="M29" s="95"/>
+      <c r="N29" s="95"/>
+      <c r="O29" s="95"/>
+      <c r="P29" s="95"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="95"/>
+      <c r="S29" s="95"/>
+      <c r="T29" s="95"/>
+      <c r="U29" s="95"/>
+      <c r="V29" s="95"/>
+      <c r="W29" s="95"/>
+      <c r="X29" s="95"/>
+      <c r="Y29" s="95"/>
+      <c r="Z29" s="95"/>
+      <c r="AA29" s="95"/>
+      <c r="AB29" s="95"/>
+      <c r="AC29" s="95"/>
+      <c r="AD29" s="95"/>
+      <c r="AE29" s="95"/>
+      <c r="AF29" s="95"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="148"/>
-      <c r="D30" s="148"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="96"/>
-      <c r="I30" s="96"/>
-      <c r="J30" s="96"/>
-      <c r="K30" s="96"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="96"/>
-      <c r="N30" s="96"/>
-      <c r="O30" s="96"/>
-      <c r="P30" s="96"/>
-      <c r="Q30" s="96"/>
-      <c r="R30" s="96"/>
-      <c r="S30" s="96"/>
-      <c r="T30" s="96"/>
-      <c r="U30" s="96"/>
-      <c r="V30" s="96"/>
-      <c r="W30" s="96"/>
-      <c r="X30" s="96"/>
-      <c r="Y30" s="96"/>
-      <c r="Z30" s="96"/>
-      <c r="AA30" s="96"/>
-      <c r="AB30" s="96"/>
-      <c r="AC30" s="96"/>
-      <c r="AD30" s="96"/>
-      <c r="AE30" s="96"/>
-      <c r="AF30" s="96"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="147"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="95"/>
+      <c r="M30" s="95"/>
+      <c r="N30" s="95"/>
+      <c r="O30" s="95"/>
+      <c r="P30" s="95"/>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="95"/>
+      <c r="S30" s="95"/>
+      <c r="T30" s="95"/>
+      <c r="U30" s="95"/>
+      <c r="V30" s="95"/>
+      <c r="W30" s="95"/>
+      <c r="X30" s="95"/>
+      <c r="Y30" s="95"/>
+      <c r="Z30" s="95"/>
+      <c r="AA30" s="95"/>
+      <c r="AB30" s="95"/>
+      <c r="AC30" s="95"/>
+      <c r="AD30" s="95"/>
+      <c r="AE30" s="95"/>
+      <c r="AF30" s="95"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="96"/>
-      <c r="I31" s="96"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="96"/>
-      <c r="M31" s="96"/>
-      <c r="N31" s="96"/>
-      <c r="O31" s="96"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="96"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="96"/>
-      <c r="U31" s="96"/>
-      <c r="V31" s="96"/>
-      <c r="W31" s="96"/>
-      <c r="X31" s="96"/>
-      <c r="Y31" s="96"/>
-      <c r="Z31" s="96"/>
-      <c r="AA31" s="96"/>
-      <c r="AB31" s="96"/>
-      <c r="AC31" s="96"/>
-      <c r="AD31" s="96"/>
-      <c r="AE31" s="96"/>
-      <c r="AF31" s="96"/>
+      <c r="C31" s="153"/>
+      <c r="D31" s="153"/>
+      <c r="G31" s="95"/>
+      <c r="H31" s="95"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="95"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="95"/>
+      <c r="M31" s="95"/>
+      <c r="N31" s="95"/>
+      <c r="O31" s="95"/>
+      <c r="P31" s="95"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="95"/>
+      <c r="T31" s="95"/>
+      <c r="U31" s="95"/>
+      <c r="V31" s="95"/>
+      <c r="W31" s="95"/>
+      <c r="X31" s="95"/>
+      <c r="Y31" s="95"/>
+      <c r="Z31" s="95"/>
+      <c r="AA31" s="95"/>
+      <c r="AB31" s="95"/>
+      <c r="AC31" s="95"/>
+      <c r="AD31" s="95"/>
+      <c r="AE31" s="95"/>
+      <c r="AF31" s="95"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="154"/>
-      <c r="D32" s="154"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="96"/>
-      <c r="I32" s="96"/>
-      <c r="J32" s="96"/>
-      <c r="K32" s="96"/>
-      <c r="L32" s="96"/>
-      <c r="M32" s="96"/>
-      <c r="N32" s="96"/>
-      <c r="O32" s="96"/>
-      <c r="P32" s="96"/>
-      <c r="Q32" s="96"/>
-      <c r="R32" s="96"/>
-      <c r="S32" s="96"/>
-      <c r="T32" s="96"/>
-      <c r="U32" s="96"/>
-      <c r="V32" s="96"/>
-      <c r="W32" s="96"/>
-      <c r="X32" s="96"/>
-      <c r="Y32" s="96"/>
-      <c r="Z32" s="96"/>
-      <c r="AA32" s="96"/>
-      <c r="AB32" s="96"/>
-      <c r="AC32" s="96"/>
-      <c r="AD32" s="96"/>
-      <c r="AE32" s="96"/>
-      <c r="AF32" s="96"/>
+      <c r="C32" s="153"/>
+      <c r="D32" s="153"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="95"/>
+      <c r="I32" s="95"/>
+      <c r="J32" s="95"/>
+      <c r="K32" s="95"/>
+      <c r="L32" s="95"/>
+      <c r="M32" s="95"/>
+      <c r="N32" s="95"/>
+      <c r="O32" s="95"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="95"/>
+      <c r="T32" s="95"/>
+      <c r="U32" s="95"/>
+      <c r="V32" s="95"/>
+      <c r="W32" s="95"/>
+      <c r="X32" s="95"/>
+      <c r="Y32" s="95"/>
+      <c r="Z32" s="95"/>
+      <c r="AA32" s="95"/>
+      <c r="AB32" s="95"/>
+      <c r="AC32" s="95"/>
+      <c r="AD32" s="95"/>
+      <c r="AE32" s="95"/>
+      <c r="AF32" s="95"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="154"/>
-      <c r="D33" s="154"/>
-      <c r="G33" s="96"/>
-      <c r="H33" s="96"/>
-      <c r="I33" s="96"/>
-      <c r="J33" s="96"/>
-      <c r="K33" s="96"/>
-      <c r="L33" s="96"/>
-      <c r="M33" s="96"/>
-      <c r="N33" s="96"/>
-      <c r="O33" s="96"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="96"/>
-      <c r="R33" s="96"/>
-      <c r="S33" s="96"/>
-      <c r="T33" s="96"/>
-      <c r="U33" s="96"/>
-      <c r="V33" s="96"/>
-      <c r="W33" s="96"/>
-      <c r="X33" s="96"/>
-      <c r="Y33" s="96"/>
-      <c r="Z33" s="96"/>
-      <c r="AA33" s="96"/>
-      <c r="AB33" s="96"/>
-      <c r="AC33" s="96"/>
-      <c r="AD33" s="96"/>
-      <c r="AE33" s="96"/>
-      <c r="AF33" s="96"/>
+      <c r="C33" s="153"/>
+      <c r="D33" s="153"/>
+      <c r="G33" s="95"/>
+      <c r="H33" s="95"/>
+      <c r="I33" s="95"/>
+      <c r="J33" s="95"/>
+      <c r="K33" s="95"/>
+      <c r="L33" s="95"/>
+      <c r="M33" s="95"/>
+      <c r="N33" s="95"/>
+      <c r="O33" s="95"/>
+      <c r="P33" s="95"/>
+      <c r="Q33" s="95"/>
+      <c r="R33" s="95"/>
+      <c r="S33" s="95"/>
+      <c r="T33" s="95"/>
+      <c r="U33" s="95"/>
+      <c r="V33" s="95"/>
+      <c r="W33" s="95"/>
+      <c r="X33" s="95"/>
+      <c r="Y33" s="95"/>
+      <c r="Z33" s="95"/>
+      <c r="AA33" s="95"/>
+      <c r="AB33" s="95"/>
+      <c r="AC33" s="95"/>
+      <c r="AD33" s="95"/>
+      <c r="AE33" s="95"/>
+      <c r="AF33" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Actualizacion del plan de proyecto anual cambio de roles
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
+++ b/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
     <sheet name="Plan Riesgos" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_2" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_4" vbProcedure="false">#ref!</definedName>
@@ -43,15 +43,16 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Sheet_Title" vbProcedure="false">"Recursos Materiales"</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Complej." vbProcedure="false">#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Sheet_Title" vbProcedure="false">"Plan Riesgos"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
@@ -160,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="235">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -513,7 +514,7 @@
     <t>Correo</t>
   </si>
   <si>
-    <t>Líder de ventas</t>
+    <t>Vendedor</t>
   </si>
   <si>
     <t>Marisol Ornelas</t>
@@ -522,9 +523,6 @@
     <t>marisol.ornelas@sos-soft.com </t>
   </si>
   <si>
-    <t>Vendedor</t>
-  </si>
-  <si>
     <t>Alma Yesenia Garcia</t>
   </si>
   <si>
@@ -540,9 +538,6 @@
     <t>zepeda.roque32@gmail.com</t>
   </si>
   <si>
-    <t>Administración</t>
-  </si>
-  <si>
     <t>Adriana Jaramillo</t>
   </si>
   <si>
@@ -574,6 +569,15 @@
   </si>
   <si>
     <t>cesar.martinez@sos-soft.com </t>
+  </si>
+  <si>
+    <t>Administracion</t>
+  </si>
+  <si>
+    <t>Magda Celene</t>
+  </si>
+  <si>
+    <t>magda.montoya@sos-soft.com</t>
   </si>
   <si>
     <t>Configuración</t>
@@ -748,16 +752,13 @@
     <t>Frecuencia de monitoreo</t>
   </si>
   <si>
-    <t>Falla de conexión remota a causa de inestabilidad de internet o incompatibilidad de software o bien no instalación en maquina cliente la cual afecta la operación de soporte</t>
-  </si>
-  <si>
-    <t>Solicitar instalación de programas adicionales como TeamViwer, Show myPC</t>
-  </si>
-  <si>
-    <t>Agendar la instalación en otra fecha disponible</t>
-  </si>
-  <si>
-    <t>Jose Francisco Llamas Diaz</t>
+    <t>Incumplimiento de procesos del modelo cmmi en ejecución</t>
+  </si>
+  <si>
+    <t>Reunión de capacitación a proceso</t>
+  </si>
+  <si>
+    <t>Reunión con dirección para validar incumplimineto</t>
   </si>
   <si>
     <t>Abierto</t>
@@ -772,61 +773,61 @@
     <t>MA</t>
   </si>
   <si>
-    <t>Problemas de instalación en maquina cliente por problemas de compatibilidad lo cual alarga la duración de proyecto</t>
-  </si>
-  <si>
-    <t>Validar los requerimientos mínimos del equipo</t>
-  </si>
-  <si>
-    <t>Buscar y ejecutar la solución, en su defecto solicitar una maquina adicional al cliente</t>
+    <t>Desviaciones en apego a procesos o productos de trabajo</t>
+  </si>
+  <si>
+    <t>Generar acciones correctivas notificando a responsable de ejecución</t>
+  </si>
+  <si>
+    <t>Escalar no conformidades con dirección</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>Falla electrica por problemas variables que afecta el uso de dispositivos, retrasando la ejecución de actividades</t>
+  </si>
+  <si>
+    <t>Comunicación con el cliente para reagendar cita</t>
+  </si>
+  <si>
+    <t>En caso de presentarse multiples días se acudira a trabajo en casa</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>El servicio de internet puede perder señal dañando la conexión y proceso de trabajo</t>
+  </si>
+  <si>
+    <t>Tener contrato con varias compañias de internet</t>
+  </si>
+  <si>
+    <t>Reportar el servicio fallido y cambiar la conexón de todas las maquinas</t>
+  </si>
+  <si>
+    <t>Presentar gasto superiores a los estimados en la cotización anual de la empresa lo cual provoca perdidas monetarias a la empresa</t>
+  </si>
+  <si>
+    <t>Contactar a todos los prospectos pendientes registrados en bitrix</t>
+  </si>
+  <si>
+    <t>Reducir horas de trabajo de empleados menos indispensables</t>
+  </si>
+  <si>
+    <t>Presentar esfuerzos superiores a los estimados en la cotización anual de la empresa lo cual provoca perdidas monetarias a la empresa</t>
+  </si>
+  <si>
+    <t>Asignar actividades a personal de otra area que este menos ocupado</t>
+  </si>
+  <si>
+    <t>Contratar personal nuevo</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>Falla de descarga de programa ocasionada por una conexión a internet limitada, la cual aumenta la duración de la tarea en soporte</t>
-  </si>
-  <si>
-    <t>Validar que la descarga se halla realizado antes de comenzar la implementación</t>
-  </si>
-  <si>
-    <t>En caso de no contar con el software descargado se descargara durante la sesión de instalación de soporte</t>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>Falla electrica por problemas variables que afecta el uso de dispositivos, retrasando la ejecución de actividades</t>
-  </si>
-  <si>
-    <t>Comunicación con el cliente para reagendar cita</t>
-  </si>
-  <si>
-    <t>En caso de presentarse multiples días se acudira a trabajo en casa</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>El servicio de internet puede perder señal dañando la conexión y proceso de trabajo</t>
-  </si>
-  <si>
-    <t>Tener contrato con varias compañias de internet</t>
-  </si>
-  <si>
-    <t>Reportar el servicio fallido y cambiar la conexón de todas las maquinas</t>
-  </si>
-  <si>
-    <t>Presentar gastos o esfuerzos superiores a los estimados en la cotización anual de la empresa lo cual provoca perdidas monetarias a la empresa</t>
-  </si>
-  <si>
-    <t>Contactar a todos los prospectos pendientes registrados en bitrix</t>
-  </si>
-  <si>
-    <t>Reducir horas de trabajo de empleados menos indispensables</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>Impacto</t>
@@ -884,7 +885,7 @@
     <numFmt numFmtId="172" formatCode="MMM\-YY"/>
     <numFmt numFmtId="173" formatCode="0%"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1088,20 +1089,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FF003366"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -1289,22 +1276,8 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
@@ -1321,6 +1294,20 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1352,7 +1339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1379,11 +1366,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="153">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1816,10 +1800,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="7" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1828,7 +1808,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1864,50 +1844,38 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1928,7 +1896,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1940,6 +1908,22 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="173" fontId="27" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1956,39 +1940,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2001,14 +1981,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2081,7 +2060,7 @@
   <dimension ref="A1:C65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="I5 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -2199,7 +2178,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="I5 C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4640,7 +4619,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+      <selection pane="topLeft" activeCell="C53" activeCellId="1" sqref="I5 C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5202,10 +5181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="I5 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5264,47 +5243,47 @@
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="64" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>121</v>
       </c>
       <c r="C5" s="64"/>
       <c r="D5" s="65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="64" t="s">
         <v>123</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>124</v>
       </c>
       <c r="C6" s="64" t="n">
         <v>3318039095</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="D7" s="65" t="s">
         <v>127</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" s="64" t="s">
         <v>7</v>
@@ -5313,66 +5292,72 @@
         <v>3312448000</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C9" s="66"/>
       <c r="D9" s="67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B10" s="67" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="66" t="n">
         <v>3316367365</v>
       </c>
       <c r="D10" s="67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" s="67" t="s">
         <v>96</v>
       </c>
       <c r="C11" s="67"/>
       <c r="D11" s="67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="67" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="68" t="s">
+      <c r="C12" s="67"/>
+      <c r="D12" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="64" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="64" t="n">
+        <v>3318039095</v>
+      </c>
+      <c r="D13" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="64" t="n">
-        <v>3318039095</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
@@ -5381,21 +5366,27 @@
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="70"/>
-      <c r="B17" s="71" t="s">
+      <c r="A16" s="69" t="s">
         <v>140</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="70"/>
+      <c r="B18" s="71" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5413,7 +5404,8 @@
     <hyperlink ref="D10" r:id="rId7" display="francisco.llamas@sos-soft.com "/>
     <hyperlink ref="B11" r:id="rId8" display="César Augusto Martínez Solís"/>
     <hyperlink ref="D11" r:id="rId9" display="cesar.martinez@sos-soft.com "/>
-    <hyperlink ref="D12" r:id="rId10" display="zepeda.roque32@gmail.com"/>
+    <hyperlink ref="D12" r:id="rId10" display="magda.montoya@sos-soft.com"/>
+    <hyperlink ref="D13" r:id="rId11" display="zepeda.roque32@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.611111111111111" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5433,7 +5425,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="I5 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5448,19 +5440,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="72" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5468,10 +5460,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D2" s="76" t="n">
         <v>42380</v>
@@ -5571,7 +5563,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D7" activeCellId="1" sqref="I5 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6653,7 +6645,7 @@
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="79" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -7681,19 +7673,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="80" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D3" s="80" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E3" s="80" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -8717,19 +8709,19 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="81" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="82" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E4" s="83" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -9753,36 +9745,36 @@
     </row>
     <row r="5" s="86" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="84" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E5" s="85" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" s="86" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="84" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B6" s="85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="82" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D6" s="82" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E6" s="85" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" s="86" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9836,7 +9828,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="1" sqref="I5 I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9864,7 +9856,7 @@
     </row>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -9875,34 +9867,34 @@
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="87" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B3" s="87" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C3" s="87" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D3" s="87" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E3" s="87" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F3" s="87" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="88" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D4" s="90" t="n">
         <v>42380</v>
@@ -9915,13 +9907,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="88" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="89" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="89" t="s">
         <v>174</v>
-      </c>
-      <c r="B5" s="89" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="89" t="s">
-        <v>173</v>
       </c>
       <c r="D5" s="90" t="n">
         <v>42380</v>
@@ -9934,13 +9926,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="88" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D6" s="90" t="n">
         <v>42380</v>
@@ -9953,13 +9945,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="88" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D7" s="90" t="n">
         <v>42380</v>
@@ -9972,13 +9964,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="88" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C8" s="89" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D8" s="90" t="n">
         <v>42380</v>
@@ -10064,10 +10056,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:JA33"/>
+  <dimension ref="A1:JA32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10132,7 +10124,7 @@
     </row>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="97" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B2" s="97"/>
       <c r="C2" s="97"/>
@@ -10166,7 +10158,7 @@
       <c r="AE2" s="0"/>
       <c r="AF2" s="0"/>
       <c r="IR2" s="98" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="IS2" s="98"/>
       <c r="IT2" s="98"/>
@@ -10210,10 +10202,10 @@
       <c r="AC3" s="0"/>
       <c r="AD3" s="0"/>
       <c r="AE3" s="99" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF3" s="99" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="IS3" s="0"/>
       <c r="IT3" s="0"/>
@@ -10226,37 +10218,37 @@
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="100" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B4" s="101" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C4" s="102" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D4" s="102" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E4" s="102" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F4" s="102" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G4" s="102" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H4" s="102" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I4" s="102" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J4" s="103" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K4" s="102" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -10278,10 +10270,10 @@
       <c r="AC4" s="0"/>
       <c r="AD4" s="0"/>
       <c r="AE4" s="104" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF4" s="104" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="IS4" s="0"/>
       <c r="IT4" s="0"/>
@@ -10292,39 +10284,39 @@
       <c r="IY4" s="0"/>
       <c r="IZ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="54.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="105" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="105" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" s="107" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="E5" s="105" t="n">
         <f aca="false">PRODUCT(A5:D5)</f>
-        <v>0.6</v>
+        <v>1.5</v>
       </c>
       <c r="F5" s="105" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="106" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H5" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="I5" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="J5" s="109" t="s">
+      <c r="I5" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="K5" s="110" t="s">
+      <c r="K5" s="109" t="s">
         <v>200</v>
       </c>
       <c r="L5" s="0"/>
@@ -10348,37 +10340,37 @@
       <c r="AD5" s="0"/>
       <c r="AE5" s="0"/>
       <c r="AF5" s="0"/>
-      <c r="IS5" s="111" t="s">
+      <c r="IS5" s="110" t="s">
         <v>201</v>
       </c>
-      <c r="IT5" s="112" t="s">
+      <c r="IT5" s="111" t="s">
         <v>202</v>
       </c>
-      <c r="IU5" s="113" t="n">
+      <c r="IU5" s="112" t="n">
         <v>0.9</v>
       </c>
-      <c r="IV5" s="114" t="n">
-        <f aca="false">(IV10*IU5)</f>
+      <c r="IV5" s="113" t="n">
+        <f aca="false">(IV9*IU5)</f>
         <v>0.9</v>
       </c>
-      <c r="IW5" s="115" t="n">
-        <f aca="false">(IW10*IU5)</f>
+      <c r="IW5" s="114" t="n">
+        <f aca="false">(IW9*IU5)</f>
         <v>1.8</v>
       </c>
-      <c r="IX5" s="116" t="n">
-        <f aca="false">(IX10*IU5)</f>
+      <c r="IX5" s="115" t="n">
+        <f aca="false">(IX9*IU5)</f>
         <v>2.7</v>
       </c>
-      <c r="IY5" s="117" t="n">
-        <f aca="false">(IY10*IU5)</f>
+      <c r="IY5" s="116" t="n">
+        <f aca="false">(IY9*IU5)</f>
         <v>3.6</v>
       </c>
-      <c r="IZ5" s="118" t="n">
-        <f aca="false">(IZ10*IU5)</f>
+      <c r="IZ5" s="117" t="n">
+        <f aca="false">(IZ9*IU5)</f>
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="105" t="n">
         <v>2</v>
       </c>
@@ -10401,16 +10393,16 @@
       <c r="G6" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="106" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="108" t="s">
-        <v>198</v>
-      </c>
-      <c r="J6" s="109" t="s">
+      <c r="I6" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="K6" s="110" t="s">
+      <c r="K6" s="109" t="s">
         <v>200</v>
       </c>
       <c r="L6" s="0"/>
@@ -10434,35 +10426,35 @@
       <c r="AD6" s="0"/>
       <c r="AE6" s="0"/>
       <c r="AF6" s="0"/>
-      <c r="IS6" s="111"/>
-      <c r="IT6" s="112" t="s">
+      <c r="IS6" s="110"/>
+      <c r="IT6" s="111" t="s">
         <v>206</v>
       </c>
-      <c r="IU6" s="113" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="IV6" s="119" t="n">
-        <f aca="false">(IV10*IU6)</f>
-        <v>0.7</v>
-      </c>
-      <c r="IW6" s="120" t="n">
-        <f aca="false">(IW10*IU6)</f>
-        <v>1.4</v>
-      </c>
-      <c r="IX6" s="121" t="n">
-        <f aca="false">(IX10*IU6)</f>
-        <v>2.1</v>
-      </c>
-      <c r="IY6" s="122" t="n">
-        <f aca="false">(IY10*IU6)</f>
-        <v>2.8</v>
-      </c>
-      <c r="IZ6" s="123" t="n">
-        <f aca="false">(IZ10*IU6)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="IU6" s="112" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="IV6" s="118" t="n">
+        <f aca="false">(IV9*IU6)</f>
+        <v>0.5</v>
+      </c>
+      <c r="IW6" s="119" t="n">
+        <f aca="false">(IW9*IU6)</f>
+        <v>1</v>
+      </c>
+      <c r="IX6" s="120" t="n">
+        <f aca="false">(IX9*IU6)</f>
+        <v>1.5</v>
+      </c>
+      <c r="IY6" s="120" t="n">
+        <f aca="false">(IY9*IU6)</f>
+        <v>2</v>
+      </c>
+      <c r="IZ6" s="121" t="n">
+        <f aca="false">(IZ9*IU6)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="105" t="n">
         <v>3</v>
       </c>
@@ -10470,17 +10462,17 @@
         <v>207</v>
       </c>
       <c r="C7" s="105" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="107" t="n">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="E7" s="105" t="n">
         <f aca="false">PRODUCT(C7:D7)</f>
-        <v>0.8</v>
+        <v>0.05</v>
       </c>
       <c r="F7" s="105" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="106" t="s">
         <v>208</v>
@@ -10489,12 +10481,12 @@
         <v>209</v>
       </c>
       <c r="I7" s="105" t="s">
-        <v>118</v>
-      </c>
-      <c r="J7" s="109" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="K7" s="110" t="s">
+      <c r="K7" s="109" t="s">
         <v>200</v>
       </c>
       <c r="L7" s="0"/>
@@ -10518,35 +10510,35 @@
       <c r="AD7" s="0"/>
       <c r="AE7" s="0"/>
       <c r="AF7" s="0"/>
-      <c r="IS7" s="111"/>
-      <c r="IT7" s="112" t="s">
+      <c r="IS7" s="110"/>
+      <c r="IT7" s="111" t="s">
         <v>210</v>
       </c>
-      <c r="IU7" s="113" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="IV7" s="119" t="n">
-        <f aca="false">(IV10*IU7)</f>
-        <v>0.5</v>
-      </c>
-      <c r="IW7" s="124" t="n">
-        <f aca="false">(IW10*IU7)</f>
-        <v>1</v>
+      <c r="IU7" s="112" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="IV7" s="122" t="n">
+        <f aca="false">(IV9*IU7)</f>
+        <v>0.3</v>
+      </c>
+      <c r="IW7" s="123" t="n">
+        <f aca="false">(IW9*IU7)</f>
+        <v>0.6</v>
       </c>
       <c r="IX7" s="120" t="n">
-        <f aca="false">(IX10*IU7)</f>
+        <f aca="false">(IX9*IU7)</f>
+        <v>0.9</v>
+      </c>
+      <c r="IY7" s="120" t="n">
+        <f aca="false">(IY9*IU7)</f>
+        <v>1.2</v>
+      </c>
+      <c r="IZ7" s="124" t="n">
+        <f aca="false">(IZ9*IU7)</f>
         <v>1.5</v>
       </c>
-      <c r="IY7" s="120" t="n">
-        <f aca="false">(IY10*IU7)</f>
-        <v>2</v>
-      </c>
-      <c r="IZ7" s="125" t="n">
-        <f aca="false">(IZ10*IU7)</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="105" t="n">
         <v>4</v>
       </c>
@@ -10557,14 +10549,14 @@
         <v>5</v>
       </c>
       <c r="D8" s="107" t="n">
-        <v>0.01</v>
+        <v>0.4</v>
       </c>
       <c r="E8" s="105" t="n">
         <f aca="false">PRODUCT(C8:D8)</f>
-        <v>0.05</v>
+        <v>2</v>
       </c>
       <c r="F8" s="105" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G8" s="106" t="s">
         <v>212</v>
@@ -10575,10 +10567,10 @@
       <c r="I8" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="109" t="s">
+      <c r="J8" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="K8" s="110" t="s">
+      <c r="K8" s="109" t="s">
         <v>200</v>
       </c>
       <c r="L8" s="0"/>
@@ -10602,67 +10594,67 @@
       <c r="AD8" s="0"/>
       <c r="AE8" s="0"/>
       <c r="AF8" s="0"/>
-      <c r="IS8" s="111"/>
-      <c r="IT8" s="112" t="s">
+      <c r="IS8" s="110"/>
+      <c r="IT8" s="111" t="s">
+        <v>206</v>
+      </c>
+      <c r="IU8" s="125" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="IV8" s="126" t="n">
+        <f aca="false">(IV9*IU8)</f>
+        <v>0.1</v>
+      </c>
+      <c r="IW8" s="127" t="n">
+        <f aca="false">(IW9*IU8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="IX8" s="128" t="n">
+        <f aca="false">(IX9*IV8)</f>
+        <v>0.3</v>
+      </c>
+      <c r="IY8" s="128" t="n">
+        <f aca="false">(IY9*IU8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="IZ8" s="129" t="n">
+        <f aca="false">(IZ9*IU8)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="130" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="106" t="s">
         <v>214</v>
-      </c>
-      <c r="IU8" s="113" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="IV8" s="126" t="n">
-        <f aca="false">(IV10*IU8)</f>
-        <v>0.3</v>
-      </c>
-      <c r="IW8" s="127" t="n">
-        <f aca="false">(IW10*IU8)</f>
-        <v>0.6</v>
-      </c>
-      <c r="IX8" s="120" t="n">
-        <f aca="false">(IX10*IU8)</f>
-        <v>0.9</v>
-      </c>
-      <c r="IY8" s="120" t="n">
-        <f aca="false">(IY10*IU8)</f>
-        <v>1.2</v>
-      </c>
-      <c r="IZ8" s="128" t="n">
-        <f aca="false">(IZ10*IU8)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="105" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="106" t="s">
-        <v>215</v>
       </c>
       <c r="C9" s="105" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="107" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="105" t="n">
         <f aca="false">PRODUCT(C9:D9)</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F9" s="105" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="106" t="s">
+        <v>215</v>
+      </c>
+      <c r="H9" s="106" t="s">
         <v>216</v>
-      </c>
-      <c r="H9" s="106" t="s">
-        <v>217</v>
       </c>
       <c r="I9" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="109" t="s">
+      <c r="J9" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="K9" s="110" t="s">
+      <c r="K9" s="109" t="s">
         <v>200</v>
       </c>
       <c r="L9" s="0"/>
@@ -10686,40 +10678,31 @@
       <c r="AD9" s="0"/>
       <c r="AE9" s="0"/>
       <c r="AF9" s="0"/>
-      <c r="IS9" s="111"/>
-      <c r="IT9" s="112" t="s">
-        <v>210</v>
-      </c>
-      <c r="IU9" s="129" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="IV9" s="130" t="n">
-        <f aca="false">(IV10*IU9)</f>
-        <v>0.1</v>
-      </c>
-      <c r="IW9" s="131" t="n">
-        <f aca="false">(IW10*IU9)</f>
-        <v>0.2</v>
-      </c>
-      <c r="IX9" s="132" t="n">
-        <f aca="false">(IX10*IV9)</f>
-        <v>0.3</v>
-      </c>
-      <c r="IY9" s="132" t="n">
-        <f aca="false">(IY10*IU9)</f>
-        <v>0.4</v>
-      </c>
-      <c r="IZ9" s="133" t="n">
-        <f aca="false">(IZ10*IU9)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="134" t="n">
+      <c r="IS9" s="131"/>
+      <c r="IT9" s="0"/>
+      <c r="IU9" s="111"/>
+      <c r="IV9" s="112" t="n">
+        <v>1</v>
+      </c>
+      <c r="IW9" s="112" t="n">
+        <v>2</v>
+      </c>
+      <c r="IX9" s="112" t="n">
+        <v>3</v>
+      </c>
+      <c r="IY9" s="112" t="n">
+        <v>4</v>
+      </c>
+      <c r="IZ9" s="132" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="133" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="106" t="s">
-        <v>218</v>
+      <c r="B10" s="134" t="s">
+        <v>217</v>
       </c>
       <c r="C10" s="105" t="n">
         <v>5</v>
@@ -10734,19 +10717,19 @@
       <c r="F10" s="105" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="106" t="s">
+      <c r="G10" s="135" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="136" t="s">
         <v>219</v>
-      </c>
-      <c r="H10" s="106" t="s">
-        <v>220</v>
       </c>
       <c r="I10" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="109" t="s">
+      <c r="J10" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="K10" s="110" t="s">
+      <c r="K10" s="137" t="s">
         <v>200</v>
       </c>
       <c r="L10" s="0"/>
@@ -10770,39 +10753,39 @@
       <c r="AD10" s="0"/>
       <c r="AE10" s="0"/>
       <c r="AF10" s="0"/>
-      <c r="IS10" s="135"/>
+      <c r="IS10" s="131"/>
       <c r="IT10" s="0"/>
-      <c r="IU10" s="112"/>
-      <c r="IV10" s="113" t="n">
-        <v>1</v>
-      </c>
-      <c r="IW10" s="113" t="n">
-        <v>2</v>
-      </c>
-      <c r="IX10" s="113" t="n">
-        <v>3</v>
-      </c>
-      <c r="IY10" s="113" t="n">
-        <v>4</v>
-      </c>
-      <c r="IZ10" s="136" t="n">
-        <v>5</v>
+      <c r="IU10" s="0"/>
+      <c r="IV10" s="111" t="s">
+        <v>206</v>
+      </c>
+      <c r="IW10" s="111" t="s">
+        <v>210</v>
+      </c>
+      <c r="IX10" s="111" t="s">
+        <v>220</v>
+      </c>
+      <c r="IY10" s="111" t="s">
+        <v>221</v>
+      </c>
+      <c r="IZ10" s="138" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="137" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="137"/>
+      <c r="A11" s="133" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="134"/>
+      <c r="C11" s="133"/>
       <c r="D11" s="139"/>
-      <c r="E11" s="137" t="n">
+      <c r="E11" s="133" t="n">
         <f aca="false">PRODUCT(C11:D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="137"/>
+      <c r="F11" s="133"/>
       <c r="G11" s="140"/>
-      <c r="H11" s="138"/>
+      <c r="H11" s="134"/>
       <c r="I11" s="141"/>
       <c r="J11" s="142"/>
       <c r="K11" s="140"/>
@@ -10827,39 +10810,31 @@
       <c r="AD11" s="0"/>
       <c r="AE11" s="0"/>
       <c r="AF11" s="0"/>
-      <c r="IS11" s="135"/>
+      <c r="IS11" s="131"/>
       <c r="IT11" s="0"/>
-      <c r="IU11" s="0"/>
-      <c r="IV11" s="112" t="s">
-        <v>210</v>
-      </c>
-      <c r="IW11" s="112" t="s">
-        <v>214</v>
-      </c>
-      <c r="IX11" s="112" t="s">
-        <v>221</v>
-      </c>
-      <c r="IY11" s="112" t="s">
-        <v>206</v>
-      </c>
-      <c r="IZ11" s="143" t="s">
-        <v>202</v>
-      </c>
+      <c r="IU11" s="112"/>
+      <c r="IV11" s="143" t="s">
+        <v>222</v>
+      </c>
+      <c r="IW11" s="143"/>
+      <c r="IX11" s="143"/>
+      <c r="IY11" s="143"/>
+      <c r="IZ11" s="143"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="137" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="137"/>
+      <c r="A12" s="133" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="134"/>
+      <c r="C12" s="133"/>
       <c r="D12" s="139"/>
-      <c r="E12" s="137" t="n">
+      <c r="E12" s="133" t="n">
         <f aca="false">PRODUCT(C12:D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="137"/>
+      <c r="F12" s="133"/>
       <c r="G12" s="140"/>
-      <c r="H12" s="138"/>
+      <c r="H12" s="134"/>
       <c r="I12" s="141"/>
       <c r="J12" s="142"/>
       <c r="K12" s="140"/>
@@ -10884,31 +10859,29 @@
       <c r="AD12" s="0"/>
       <c r="AE12" s="0"/>
       <c r="AF12" s="0"/>
-      <c r="IS12" s="135"/>
+      <c r="IS12" s="131"/>
       <c r="IT12" s="0"/>
-      <c r="IU12" s="113"/>
-      <c r="IV12" s="144" t="s">
-        <v>222</v>
-      </c>
-      <c r="IW12" s="144"/>
-      <c r="IX12" s="144"/>
-      <c r="IY12" s="144"/>
+      <c r="IU12" s="0"/>
+      <c r="IV12" s="0"/>
+      <c r="IW12" s="0"/>
+      <c r="IX12" s="0"/>
+      <c r="IY12" s="0"/>
       <c r="IZ12" s="144"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="137" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="138"/>
-      <c r="C13" s="137"/>
+      <c r="A13" s="133" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="134"/>
+      <c r="C13" s="133"/>
       <c r="D13" s="139"/>
-      <c r="E13" s="137" t="n">
+      <c r="E13" s="133" t="n">
         <f aca="false">PRODUCT(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="137"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="140"/>
-      <c r="H13" s="138"/>
+      <c r="H13" s="134"/>
       <c r="I13" s="141"/>
       <c r="J13" s="142"/>
       <c r="K13" s="140"/>
@@ -10933,32 +10906,27 @@
       <c r="AD13" s="0"/>
       <c r="AE13" s="0"/>
       <c r="AF13" s="0"/>
-      <c r="IS13" s="135"/>
+      <c r="IS13" s="131"/>
       <c r="IT13" s="0"/>
-      <c r="IU13" s="0"/>
-      <c r="IV13" s="0"/>
-      <c r="IW13" s="0"/>
-      <c r="IX13" s="0"/>
-      <c r="IY13" s="0"/>
+      <c r="IU13" s="104"/>
+      <c r="IV13" s="104"/>
+      <c r="IW13" s="104"/>
+      <c r="IX13" s="104"/>
+      <c r="IY13" s="104"/>
       <c r="IZ13" s="145"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="137" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" s="138"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="139"/>
-      <c r="E14" s="137" t="n">
-        <f aca="false">PRODUCT(C14:D14)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="137"/>
-      <c r="G14" s="140"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="141"/>
-      <c r="J14" s="142"/>
-      <c r="K14" s="140"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="146"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="146"/>
+      <c r="F14" s="146"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
@@ -10980,22 +10948,14 @@
       <c r="AD14" s="0"/>
       <c r="AE14" s="0"/>
       <c r="AF14" s="0"/>
-      <c r="IS14" s="135"/>
-      <c r="IT14" s="0"/>
-      <c r="IU14" s="104"/>
-      <c r="IV14" s="104"/>
-      <c r="IW14" s="104"/>
-      <c r="IX14" s="104"/>
-      <c r="IY14" s="104"/>
-      <c r="IZ14" s="146"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="147"/>
-      <c r="B15" s="147"/>
-      <c r="C15" s="147"/>
-      <c r="D15" s="147"/>
-      <c r="E15" s="147"/>
-      <c r="F15" s="147"/>
+      <c r="A15" s="146"/>
+      <c r="B15" s="146"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="146"/>
+      <c r="F15" s="146"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
@@ -11024,12 +10984,12 @@
       <c r="AF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="147"/>
-      <c r="B16" s="147"/>
-      <c r="C16" s="147"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="147"/>
+      <c r="A16" s="146"/>
+      <c r="B16" s="146"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="146"/>
+      <c r="F16" s="146"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -11057,13 +11017,15 @@
       <c r="AE16" s="0"/>
       <c r="AF16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="147"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="147" t="s">
+        <v>223</v>
+      </c>
       <c r="B17" s="147"/>
       <c r="C17" s="147"/>
-      <c r="D17" s="147"/>
-      <c r="E17" s="147"/>
-      <c r="F17" s="147"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -11091,15 +11053,19 @@
       <c r="AE17" s="0"/>
       <c r="AF17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="148" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" s="148"/>
-      <c r="C18" s="148"/>
-      <c r="D18" s="147"/>
-      <c r="E18" s="147"/>
-      <c r="F18" s="147"/>
+        <v>224</v>
+      </c>
+      <c r="B18" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" s="148" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" s="146"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -11127,19 +11093,19 @@
       <c r="AE18" s="0"/>
       <c r="AF18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="149" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="150" t="s">
-        <v>225</v>
-      </c>
-      <c r="C19" s="149" t="s">
-        <v>226</v>
-      </c>
-      <c r="D19" s="147"/>
-      <c r="E19" s="147"/>
-      <c r="F19" s="147"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="148" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="148" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19" s="150"/>
+      <c r="E19" s="150"/>
+      <c r="F19" s="146"/>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -11168,18 +11134,16 @@
       <c r="AF19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="149" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="149" t="s">
-        <v>227</v>
-      </c>
-      <c r="C20" s="149" t="s">
-        <v>228</v>
-      </c>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="147"/>
+      <c r="A20" s="151" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="151" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="151" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="0"/>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -11208,14 +11172,14 @@
       <c r="AF20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="152" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" s="152" t="s">
-        <v>229</v>
-      </c>
-      <c r="C21" s="152" t="s">
-        <v>230</v>
+      <c r="A21" s="151" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="151" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="151" t="s">
+        <v>232</v>
       </c>
       <c r="D21" s="0"/>
       <c r="G21" s="0"/>
@@ -11246,14 +11210,14 @@
       <c r="AF21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="152" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="152" t="s">
-        <v>231</v>
-      </c>
-      <c r="C22" s="152" t="s">
-        <v>232</v>
+      <c r="A22" s="151" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="151" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" s="151" t="s">
+        <v>234</v>
       </c>
       <c r="D22" s="0"/>
       <c r="G22" s="0"/>
@@ -11283,16 +11247,8 @@
       <c r="AE22" s="0"/>
       <c r="AF22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="152" t="n">
-        <v>4</v>
-      </c>
-      <c r="B23" s="152" t="s">
-        <v>233</v>
-      </c>
-      <c r="C23" s="152" t="s">
-        <v>234</v>
-      </c>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0"/>
       <c r="D23" s="0"/>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
@@ -11412,38 +11368,38 @@
       <c r="AF26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
-      <c r="J27" s="0"/>
-      <c r="K27" s="0"/>
-      <c r="L27" s="0"/>
-      <c r="M27" s="0"/>
-      <c r="N27" s="0"/>
-      <c r="O27" s="0"/>
-      <c r="P27" s="0"/>
-      <c r="Q27" s="0"/>
-      <c r="R27" s="0"/>
-      <c r="S27" s="0"/>
-      <c r="T27" s="0"/>
-      <c r="U27" s="0"/>
-      <c r="V27" s="0"/>
-      <c r="W27" s="0"/>
-      <c r="X27" s="0"/>
-      <c r="Y27" s="0"/>
-      <c r="Z27" s="0"/>
-      <c r="AA27" s="0"/>
-      <c r="AB27" s="0"/>
-      <c r="AC27" s="0"/>
-      <c r="AD27" s="0"/>
-      <c r="AE27" s="0"/>
-      <c r="AF27" s="0"/>
+      <c r="C27" s="146"/>
+      <c r="D27" s="146"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="95"/>
+      <c r="M27" s="95"/>
+      <c r="N27" s="95"/>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="95"/>
+      <c r="T27" s="95"/>
+      <c r="U27" s="95"/>
+      <c r="V27" s="95"/>
+      <c r="W27" s="95"/>
+      <c r="X27" s="95"/>
+      <c r="Y27" s="95"/>
+      <c r="Z27" s="95"/>
+      <c r="AA27" s="95"/>
+      <c r="AB27" s="95"/>
+      <c r="AC27" s="95"/>
+      <c r="AD27" s="95"/>
+      <c r="AE27" s="95"/>
+      <c r="AF27" s="95"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="147"/>
-      <c r="D28" s="147"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
       <c r="G28" s="95"/>
       <c r="H28" s="95"/>
       <c r="I28" s="95"/>
@@ -11472,8 +11428,8 @@
       <c r="AF28" s="95"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="147"/>
-      <c r="D29" s="147"/>
+      <c r="C29" s="146"/>
+      <c r="D29" s="146"/>
       <c r="G29" s="95"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
@@ -11502,8 +11458,8 @@
       <c r="AF29" s="95"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="147"/>
-      <c r="D30" s="147"/>
+      <c r="C30" s="152"/>
+      <c r="D30" s="152"/>
       <c r="G30" s="95"/>
       <c r="H30" s="95"/>
       <c r="I30" s="95"/>
@@ -11532,8 +11488,8 @@
       <c r="AF30" s="95"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="153"/>
-      <c r="D31" s="153"/>
+      <c r="C31" s="152"/>
+      <c r="D31" s="152"/>
       <c r="G31" s="95"/>
       <c r="H31" s="95"/>
       <c r="I31" s="95"/>
@@ -11562,8 +11518,8 @@
       <c r="AF31" s="95"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="153"/>
-      <c r="D32" s="153"/>
+      <c r="C32" s="152"/>
+      <c r="D32" s="152"/>
       <c r="G32" s="95"/>
       <c r="H32" s="95"/>
       <c r="I32" s="95"/>
@@ -11591,51 +11547,21 @@
       <c r="AE32" s="95"/>
       <c r="AF32" s="95"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="153"/>
-      <c r="D33" s="153"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
-      <c r="K33" s="95"/>
-      <c r="L33" s="95"/>
-      <c r="M33" s="95"/>
-      <c r="N33" s="95"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="95"/>
-      <c r="S33" s="95"/>
-      <c r="T33" s="95"/>
-      <c r="U33" s="95"/>
-      <c r="V33" s="95"/>
-      <c r="W33" s="95"/>
-      <c r="X33" s="95"/>
-      <c r="Y33" s="95"/>
-      <c r="Z33" s="95"/>
-      <c r="AA33" s="95"/>
-      <c r="AB33" s="95"/>
-      <c r="AC33" s="95"/>
-      <c r="AD33" s="95"/>
-      <c r="AE33" s="95"/>
-      <c r="AF33" s="95"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:K3"/>
-    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:C9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:C8" type="list">
       <formula1>",1,2,3,4,5"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F9" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F8" type="list">
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J5:J8" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J5:J7" type="list">
       <formula1>"Abierto,Mitigado,Ocurrido,Cerrado"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Actualizacón integrantes equipo plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
+++ b/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,6 +53,8 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Sheet_Title" vbProcedure="false">"Plan Riesgos"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
@@ -161,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="242">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -499,6 +501,30 @@
     <t>La estimación de esfuerzo esta basada en el número de proyectos esperados para poder alcanzar la meta de ventas establecida anualmente por la empresa</t>
   </si>
   <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Número de tickets</t>
+  </si>
+  <si>
+    <t>Valor estimado promedio</t>
+  </si>
+  <si>
+    <t>Tickets mensuales</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>3360 pesos en promedio por ticket</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>Se estima un promedio del 80 por ciento de asistencia de soporte para las ventas generadas por el area de ventas de las cuales al mes se esperan 40 tickets con una duracion entre 1 y dos horas y el resto superior a esas dos horas.</t>
+  </si>
+  <si>
     <t>Matriz de responsabilidades</t>
   </si>
   <si>
@@ -551,9 +577,6 @@
   </si>
   <si>
     <t>r.novela@sos-soft.com</t>
-  </si>
-  <si>
-    <t>Soporte</t>
   </si>
   <si>
     <t>Francisco gonzales Sanchez</t>
@@ -1367,7 +1390,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="158">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1610,6 +1633,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2060,7 +2103,7 @@
   <dimension ref="A1:C65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="I5 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -2178,7 +2221,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="I5 C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4616,10 +4659,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="1" sqref="I5 C53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5151,6 +5194,49 @@
         <v>111</v>
       </c>
       <c r="B63" s="60"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="D64" s="62" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" s="63" t="n">
+        <v>960</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D65" s="64" t="n">
+        <f aca="false">960/12</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="63" t="n">
+        <v>750</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66" s="65" t="n">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5184,7 +5270,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="I5 C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5198,165 +5284,165 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="A1" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="A2" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="63" t="s">
+      <c r="A3" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="63" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="63" t="s">
-        <v>116</v>
+      <c r="C3" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="64" t="s">
+      <c r="A4" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="69" t="n">
+        <v>3313482553</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="70" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="69" t="n">
+        <v>3318039095</v>
+      </c>
+      <c r="D6" s="70" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="69" t="n">
+        <v>3312448000</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="64" t="n">
-        <v>3313482553</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="64" t="n">
+      <c r="B9" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="71" t="n">
+        <v>3316367365</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="72"/>
+      <c r="D12" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="69" t="n">
         <v>3318039095</v>
       </c>
-      <c r="D6" s="65" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="64" t="n">
-        <v>3312448000</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67" t="s">
+      <c r="D13" s="70" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="66" t="n">
-        <v>3316367365</v>
-      </c>
-      <c r="D10" s="67" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="67" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="66" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="64" t="n">
-        <v>3318039095</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5372,21 +5458,21 @@
       <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="A16" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="70"/>
-      <c r="B18" s="71" t="s">
-        <v>141</v>
+      <c r="A18" s="75"/>
+      <c r="B18" s="76" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -5425,7 +5511,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="I5 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5439,108 +5525,108 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="73" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="73" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="74" t="n">
+      <c r="A1" s="77" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="85.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="79" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="75" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="76" t="n">
+        <v>154</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="81" t="n">
         <v>42380</v>
       </c>
-      <c r="E2" s="76" t="n">
+      <c r="E2" s="81" t="n">
         <v>42380</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="77"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="77"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5563,7 +5649,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D7" activeCellId="1" sqref="I5 D7"/>
+      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6644,13 +6730,13 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="79" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
+      <c r="A2" s="84" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -7672,20 +7758,20 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="85" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" s="80" t="s">
-        <v>153</v>
+      <c r="D3" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="85" t="s">
+        <v>160</v>
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -8708,20 +8794,20 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="81" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="81" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="82" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="82" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="83" t="s">
-        <v>157</v>
+      <c r="A4" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>164</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -9743,67 +9829,67 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="86" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="84" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="82" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="82" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="85" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" s="86" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="82" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="82" t="s">
-        <v>163</v>
-      </c>
-      <c r="E6" s="85" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" s="86" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="84"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="85"/>
-    </row>
-    <row r="8" s="86" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="85"/>
+    <row r="5" s="91" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="87" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="90" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" s="91" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="89" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="90" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" s="91" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="89"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="90"/>
+    </row>
+    <row r="8" s="91" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="90"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="84"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="84"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9828,7 +9914,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="1" sqref="I5 I8"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9856,7 +9942,7 @@
     </row>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -9866,175 +9952,175 @@
       <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="87" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" s="87" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="87" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" s="87" t="s">
-        <v>171</v>
+      <c r="A3" s="92" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="92" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="92" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="92" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="92" t="s">
+        <v>178</v>
       </c>
       <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="88" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="89" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="89" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="90" t="n">
+      <c r="A4" s="93" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="95" t="n">
         <v>42380</v>
       </c>
-      <c r="E4" s="90" t="n">
+      <c r="E4" s="95" t="n">
         <v>42373</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="I4" s="91"/>
+      <c r="F4" s="94"/>
+      <c r="I4" s="96"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="88" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="89" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="89" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="90" t="n">
+      <c r="A5" s="93" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="95" t="n">
         <v>42380</v>
       </c>
-      <c r="E5" s="90" t="n">
+      <c r="E5" s="95" t="n">
         <v>42373</v>
       </c>
-      <c r="F5" s="89"/>
-      <c r="I5" s="91"/>
+      <c r="F5" s="94"/>
+      <c r="I5" s="96"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="88" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" s="89" t="s">
-        <v>177</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="90" t="n">
+      <c r="A6" s="93" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="95" t="n">
         <v>42380</v>
       </c>
-      <c r="E6" s="90" t="n">
+      <c r="E6" s="95" t="n">
         <v>42373</v>
       </c>
-      <c r="F6" s="89"/>
-      <c r="I6" s="91"/>
+      <c r="F6" s="94"/>
+      <c r="I6" s="96"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="88" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="89" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="89" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" s="90" t="n">
+      <c r="A7" s="93" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="95" t="n">
         <v>42380</v>
       </c>
-      <c r="E7" s="90" t="n">
+      <c r="E7" s="95" t="n">
         <v>42373</v>
       </c>
-      <c r="F7" s="89"/>
-      <c r="I7" s="91"/>
+      <c r="F7" s="94"/>
+      <c r="I7" s="96"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="93" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="89" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="89" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="90" t="n">
+      <c r="C8" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="95" t="n">
         <v>42380</v>
       </c>
-      <c r="E8" s="90" t="n">
+      <c r="E8" s="95" t="n">
         <v>42373</v>
       </c>
-      <c r="F8" s="89"/>
+      <c r="F8" s="94"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="92"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="89"/>
+      <c r="A9" s="97"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="94"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="88"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="89"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="94"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="89"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="94"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="88"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="89"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="94"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10058,7 +10144,7 @@
   </sheetPr>
   <dimension ref="A1:JA32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -10079,10 +10165,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="95"/>
+      <c r="A1" s="100"/>
       <c r="B1" s="0"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -10123,19 +10209,19 @@
       <c r="JA1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="97" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="A2" s="102" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
@@ -10157,31 +10243,31 @@
       <c r="AD2" s="0"/>
       <c r="AE2" s="0"/>
       <c r="AF2" s="0"/>
-      <c r="IR2" s="98" t="s">
-        <v>182</v>
-      </c>
-      <c r="IS2" s="98"/>
-      <c r="IT2" s="98"/>
-      <c r="IU2" s="98"/>
-      <c r="IV2" s="98"/>
-      <c r="IW2" s="98"/>
-      <c r="IX2" s="98"/>
-      <c r="IY2" s="98"/>
-      <c r="IZ2" s="98"/>
-      <c r="JA2" s="98"/>
+      <c r="IR2" s="103" t="s">
+        <v>189</v>
+      </c>
+      <c r="IS2" s="103"/>
+      <c r="IT2" s="103"/>
+      <c r="IU2" s="103"/>
+      <c r="IV2" s="103"/>
+      <c r="IW2" s="103"/>
+      <c r="IX2" s="103"/>
+      <c r="IY2" s="103"/>
+      <c r="IZ2" s="103"/>
+      <c r="JA2" s="103"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="97"/>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
@@ -10201,11 +10287,11 @@
       <c r="AB3" s="0"/>
       <c r="AC3" s="0"/>
       <c r="AD3" s="0"/>
-      <c r="AE3" s="99" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF3" s="99" t="s">
-        <v>184</v>
+      <c r="AE3" s="104" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF3" s="104" t="s">
+        <v>191</v>
       </c>
       <c r="IS3" s="0"/>
       <c r="IT3" s="0"/>
@@ -10217,38 +10303,38 @@
       <c r="IZ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="100" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="101" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="102" t="s">
-        <v>187</v>
-      </c>
-      <c r="D4" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="E4" s="102" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" s="102" t="s">
-        <v>190</v>
-      </c>
-      <c r="G4" s="102" t="s">
-        <v>191</v>
-      </c>
-      <c r="H4" s="102" t="s">
+      <c r="A4" s="105" t="s">
         <v>192</v>
       </c>
-      <c r="I4" s="102" t="s">
+      <c r="B4" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="J4" s="103" t="s">
+      <c r="C4" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="K4" s="102" t="s">
+      <c r="D4" s="107" t="s">
         <v>195</v>
+      </c>
+      <c r="E4" s="107" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="107" t="s">
+        <v>197</v>
+      </c>
+      <c r="G4" s="107" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="I4" s="107" t="s">
+        <v>200</v>
+      </c>
+      <c r="J4" s="108" t="s">
+        <v>201</v>
+      </c>
+      <c r="K4" s="107" t="s">
+        <v>202</v>
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -10269,11 +10355,11 @@
       <c r="AB4" s="0"/>
       <c r="AC4" s="0"/>
       <c r="AD4" s="0"/>
-      <c r="AE4" s="104" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF4" s="104" t="s">
-        <v>184</v>
+      <c r="AE4" s="109" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF4" s="109" t="s">
+        <v>191</v>
       </c>
       <c r="IS4" s="0"/>
       <c r="IT4" s="0"/>
@@ -10285,39 +10371,39 @@
       <c r="IZ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="54.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="105" t="n">
+      <c r="A5" s="110" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="106" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="105" t="n">
+      <c r="B5" s="111" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="107" t="n">
+      <c r="D5" s="112" t="n">
         <v>0.3</v>
       </c>
-      <c r="E5" s="105" t="n">
+      <c r="E5" s="110" t="n">
         <f aca="false">PRODUCT(A5:D5)</f>
         <v>1.5</v>
       </c>
-      <c r="F5" s="105" t="n">
+      <c r="F5" s="110" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="106" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="108" t="s">
-        <v>199</v>
-      </c>
-      <c r="K5" s="109" t="s">
-        <v>200</v>
+      <c r="G5" s="111" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="111" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="J5" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" s="114" t="s">
+        <v>207</v>
       </c>
       <c r="L5" s="0"/>
       <c r="M5" s="0"/>
@@ -10340,70 +10426,70 @@
       <c r="AD5" s="0"/>
       <c r="AE5" s="0"/>
       <c r="AF5" s="0"/>
-      <c r="IS5" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="IT5" s="111" t="s">
-        <v>202</v>
-      </c>
-      <c r="IU5" s="112" t="n">
+      <c r="IS5" s="115" t="s">
+        <v>208</v>
+      </c>
+      <c r="IT5" s="116" t="s">
+        <v>209</v>
+      </c>
+      <c r="IU5" s="117" t="n">
         <v>0.9</v>
       </c>
-      <c r="IV5" s="113" t="n">
+      <c r="IV5" s="118" t="n">
         <f aca="false">(IV9*IU5)</f>
         <v>0.9</v>
       </c>
-      <c r="IW5" s="114" t="n">
+      <c r="IW5" s="119" t="n">
         <f aca="false">(IW9*IU5)</f>
         <v>1.8</v>
       </c>
-      <c r="IX5" s="115" t="n">
+      <c r="IX5" s="120" t="n">
         <f aca="false">(IX9*IU5)</f>
         <v>2.7</v>
       </c>
-      <c r="IY5" s="116" t="n">
+      <c r="IY5" s="121" t="n">
         <f aca="false">(IY9*IU5)</f>
         <v>3.6</v>
       </c>
-      <c r="IZ5" s="117" t="n">
+      <c r="IZ5" s="122" t="n">
         <f aca="false">(IZ9*IU5)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="105" t="n">
+      <c r="A6" s="110" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="106" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="105" t="n">
+      <c r="B6" s="111" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="110" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="107" t="n">
+      <c r="D6" s="112" t="n">
         <v>0.2</v>
       </c>
-      <c r="E6" s="105" t="n">
+      <c r="E6" s="110" t="n">
         <f aca="false">PRODUCT(C6:D6)</f>
         <v>0.8</v>
       </c>
-      <c r="F6" s="105" t="n">
+      <c r="F6" s="110" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="106" t="s">
-        <v>204</v>
-      </c>
-      <c r="H6" s="106" t="s">
-        <v>205</v>
-      </c>
-      <c r="I6" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="J6" s="108" t="s">
-        <v>199</v>
-      </c>
-      <c r="K6" s="109" t="s">
-        <v>200</v>
+      <c r="G6" s="111" t="s">
+        <v>211</v>
+      </c>
+      <c r="H6" s="111" t="s">
+        <v>212</v>
+      </c>
+      <c r="I6" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="K6" s="114" t="s">
+        <v>207</v>
       </c>
       <c r="L6" s="0"/>
       <c r="M6" s="0"/>
@@ -10426,68 +10512,68 @@
       <c r="AD6" s="0"/>
       <c r="AE6" s="0"/>
       <c r="AF6" s="0"/>
-      <c r="IS6" s="110"/>
-      <c r="IT6" s="111" t="s">
-        <v>206</v>
-      </c>
-      <c r="IU6" s="112" t="n">
+      <c r="IS6" s="115"/>
+      <c r="IT6" s="116" t="s">
+        <v>213</v>
+      </c>
+      <c r="IU6" s="117" t="n">
         <v>0.5</v>
       </c>
-      <c r="IV6" s="118" t="n">
+      <c r="IV6" s="123" t="n">
         <f aca="false">(IV9*IU6)</f>
         <v>0.5</v>
       </c>
-      <c r="IW6" s="119" t="n">
+      <c r="IW6" s="124" t="n">
         <f aca="false">(IW9*IU6)</f>
         <v>1</v>
       </c>
-      <c r="IX6" s="120" t="n">
+      <c r="IX6" s="125" t="n">
         <f aca="false">(IX9*IU6)</f>
         <v>1.5</v>
       </c>
-      <c r="IY6" s="120" t="n">
+      <c r="IY6" s="125" t="n">
         <f aca="false">(IY9*IU6)</f>
         <v>2</v>
       </c>
-      <c r="IZ6" s="121" t="n">
+      <c r="IZ6" s="126" t="n">
         <f aca="false">(IZ9*IU6)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="105" t="n">
+      <c r="A7" s="110" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="106" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="105" t="n">
+      <c r="B7" s="111" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="107" t="n">
+      <c r="D7" s="112" t="n">
         <v>0.01</v>
       </c>
-      <c r="E7" s="105" t="n">
+      <c r="E7" s="110" t="n">
         <f aca="false">PRODUCT(C7:D7)</f>
         <v>0.05</v>
       </c>
-      <c r="F7" s="105" t="n">
+      <c r="F7" s="110" t="n">
         <v>4</v>
       </c>
-      <c r="G7" s="106" t="s">
-        <v>208</v>
-      </c>
-      <c r="H7" s="106" t="s">
-        <v>209</v>
-      </c>
-      <c r="I7" s="105" t="s">
+      <c r="G7" s="111" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="111" t="s">
+        <v>216</v>
+      </c>
+      <c r="I7" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="108" t="s">
-        <v>199</v>
-      </c>
-      <c r="K7" s="109" t="s">
-        <v>200</v>
+      <c r="J7" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="K7" s="114" t="s">
+        <v>207</v>
       </c>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -10510,68 +10596,68 @@
       <c r="AD7" s="0"/>
       <c r="AE7" s="0"/>
       <c r="AF7" s="0"/>
-      <c r="IS7" s="110"/>
-      <c r="IT7" s="111" t="s">
-        <v>210</v>
-      </c>
-      <c r="IU7" s="112" t="n">
+      <c r="IS7" s="115"/>
+      <c r="IT7" s="116" t="s">
+        <v>217</v>
+      </c>
+      <c r="IU7" s="117" t="n">
         <v>0.3</v>
       </c>
-      <c r="IV7" s="122" t="n">
+      <c r="IV7" s="127" t="n">
         <f aca="false">(IV9*IU7)</f>
         <v>0.3</v>
       </c>
-      <c r="IW7" s="123" t="n">
+      <c r="IW7" s="128" t="n">
         <f aca="false">(IW9*IU7)</f>
         <v>0.6</v>
       </c>
-      <c r="IX7" s="120" t="n">
+      <c r="IX7" s="125" t="n">
         <f aca="false">(IX9*IU7)</f>
         <v>0.9</v>
       </c>
-      <c r="IY7" s="120" t="n">
+      <c r="IY7" s="125" t="n">
         <f aca="false">(IY9*IU7)</f>
         <v>1.2</v>
       </c>
-      <c r="IZ7" s="124" t="n">
+      <c r="IZ7" s="129" t="n">
         <f aca="false">(IZ9*IU7)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="105" t="n">
+      <c r="A8" s="110" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="106" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="105" t="n">
+      <c r="B8" s="111" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="107" t="n">
+      <c r="D8" s="112" t="n">
         <v>0.4</v>
       </c>
-      <c r="E8" s="105" t="n">
+      <c r="E8" s="110" t="n">
         <f aca="false">PRODUCT(C8:D8)</f>
         <v>2</v>
       </c>
-      <c r="F8" s="105" t="n">
+      <c r="F8" s="110" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="106" t="s">
-        <v>212</v>
-      </c>
-      <c r="H8" s="106" t="s">
-        <v>213</v>
-      </c>
-      <c r="I8" s="105" t="s">
+      <c r="G8" s="111" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="111" t="s">
+        <v>220</v>
+      </c>
+      <c r="I8" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="108" t="s">
-        <v>199</v>
-      </c>
-      <c r="K8" s="109" t="s">
-        <v>200</v>
+      <c r="J8" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="K8" s="114" t="s">
+        <v>207</v>
       </c>
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
@@ -10594,68 +10680,68 @@
       <c r="AD8" s="0"/>
       <c r="AE8" s="0"/>
       <c r="AF8" s="0"/>
-      <c r="IS8" s="110"/>
-      <c r="IT8" s="111" t="s">
-        <v>206</v>
-      </c>
-      <c r="IU8" s="125" t="n">
+      <c r="IS8" s="115"/>
+      <c r="IT8" s="116" t="s">
+        <v>213</v>
+      </c>
+      <c r="IU8" s="130" t="n">
         <v>0.1</v>
       </c>
-      <c r="IV8" s="126" t="n">
+      <c r="IV8" s="131" t="n">
         <f aca="false">(IV9*IU8)</f>
         <v>0.1</v>
       </c>
-      <c r="IW8" s="127" t="n">
+      <c r="IW8" s="132" t="n">
         <f aca="false">(IW9*IU8)</f>
         <v>0.2</v>
       </c>
-      <c r="IX8" s="128" t="n">
+      <c r="IX8" s="133" t="n">
         <f aca="false">(IX9*IV8)</f>
         <v>0.3</v>
       </c>
-      <c r="IY8" s="128" t="n">
+      <c r="IY8" s="133" t="n">
         <f aca="false">(IY9*IU8)</f>
         <v>0.4</v>
       </c>
-      <c r="IZ8" s="129" t="n">
+      <c r="IZ8" s="134" t="n">
         <f aca="false">(IZ9*IU8)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="130" t="n">
+      <c r="A9" s="135" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="106" t="s">
-        <v>214</v>
-      </c>
-      <c r="C9" s="105" t="n">
+      <c r="B9" s="111" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="107" t="n">
+      <c r="D9" s="112" t="n">
         <v>0.2</v>
       </c>
-      <c r="E9" s="105" t="n">
+      <c r="E9" s="110" t="n">
         <f aca="false">PRODUCT(C9:D9)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="105" t="n">
+      <c r="F9" s="110" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="106" t="s">
-        <v>215</v>
-      </c>
-      <c r="H9" s="106" t="s">
-        <v>216</v>
-      </c>
-      <c r="I9" s="105" t="s">
+      <c r="G9" s="111" t="s">
+        <v>222</v>
+      </c>
+      <c r="H9" s="111" t="s">
+        <v>223</v>
+      </c>
+      <c r="I9" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="108" t="s">
-        <v>199</v>
-      </c>
-      <c r="K9" s="109" t="s">
-        <v>200</v>
+      <c r="J9" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="K9" s="114" t="s">
+        <v>207</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
@@ -10678,59 +10764,59 @@
       <c r="AD9" s="0"/>
       <c r="AE9" s="0"/>
       <c r="AF9" s="0"/>
-      <c r="IS9" s="131"/>
+      <c r="IS9" s="136"/>
       <c r="IT9" s="0"/>
-      <c r="IU9" s="111"/>
-      <c r="IV9" s="112" t="n">
+      <c r="IU9" s="116"/>
+      <c r="IV9" s="117" t="n">
         <v>1</v>
       </c>
-      <c r="IW9" s="112" t="n">
+      <c r="IW9" s="117" t="n">
         <v>2</v>
       </c>
-      <c r="IX9" s="112" t="n">
+      <c r="IX9" s="117" t="n">
         <v>3</v>
       </c>
-      <c r="IY9" s="112" t="n">
+      <c r="IY9" s="117" t="n">
         <v>4</v>
       </c>
-      <c r="IZ9" s="132" t="n">
+      <c r="IZ9" s="137" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="133" t="n">
+      <c r="A10" s="138" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="134" t="s">
-        <v>217</v>
-      </c>
-      <c r="C10" s="105" t="n">
+      <c r="B10" s="139" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="107" t="n">
+      <c r="D10" s="112" t="n">
         <v>0.2</v>
       </c>
-      <c r="E10" s="105" t="n">
+      <c r="E10" s="110" t="n">
         <f aca="false">PRODUCT(C10:D10)</f>
         <v>1</v>
       </c>
-      <c r="F10" s="105" t="n">
+      <c r="F10" s="110" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="135" t="s">
-        <v>218</v>
-      </c>
-      <c r="H10" s="136" t="s">
-        <v>219</v>
-      </c>
-      <c r="I10" s="105" t="s">
+      <c r="G10" s="140" t="s">
+        <v>225</v>
+      </c>
+      <c r="H10" s="141" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="108" t="s">
-        <v>199</v>
-      </c>
-      <c r="K10" s="137" t="s">
-        <v>200</v>
+      <c r="J10" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="K10" s="142" t="s">
+        <v>207</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
@@ -10753,42 +10839,42 @@
       <c r="AD10" s="0"/>
       <c r="AE10" s="0"/>
       <c r="AF10" s="0"/>
-      <c r="IS10" s="131"/>
+      <c r="IS10" s="136"/>
       <c r="IT10" s="0"/>
       <c r="IU10" s="0"/>
-      <c r="IV10" s="111" t="s">
-        <v>206</v>
-      </c>
-      <c r="IW10" s="111" t="s">
-        <v>210</v>
-      </c>
-      <c r="IX10" s="111" t="s">
-        <v>220</v>
-      </c>
-      <c r="IY10" s="111" t="s">
-        <v>221</v>
-      </c>
-      <c r="IZ10" s="138" t="s">
-        <v>202</v>
+      <c r="IV10" s="116" t="s">
+        <v>213</v>
+      </c>
+      <c r="IW10" s="116" t="s">
+        <v>217</v>
+      </c>
+      <c r="IX10" s="116" t="s">
+        <v>227</v>
+      </c>
+      <c r="IY10" s="116" t="s">
+        <v>228</v>
+      </c>
+      <c r="IZ10" s="143" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="133" t="n">
+      <c r="A11" s="138" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="134"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="139"/>
-      <c r="E11" s="133" t="n">
+      <c r="B11" s="139"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="138" t="n">
         <f aca="false">PRODUCT(C11:D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="133"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="134"/>
-      <c r="I11" s="141"/>
-      <c r="J11" s="142"/>
-      <c r="K11" s="140"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="139"/>
+      <c r="I11" s="146"/>
+      <c r="J11" s="147"/>
+      <c r="K11" s="145"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
@@ -10810,34 +10896,34 @@
       <c r="AD11" s="0"/>
       <c r="AE11" s="0"/>
       <c r="AF11" s="0"/>
-      <c r="IS11" s="131"/>
+      <c r="IS11" s="136"/>
       <c r="IT11" s="0"/>
-      <c r="IU11" s="112"/>
-      <c r="IV11" s="143" t="s">
-        <v>222</v>
-      </c>
-      <c r="IW11" s="143"/>
-      <c r="IX11" s="143"/>
-      <c r="IY11" s="143"/>
-      <c r="IZ11" s="143"/>
+      <c r="IU11" s="117"/>
+      <c r="IV11" s="148" t="s">
+        <v>229</v>
+      </c>
+      <c r="IW11" s="148"/>
+      <c r="IX11" s="148"/>
+      <c r="IY11" s="148"/>
+      <c r="IZ11" s="148"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="133" t="n">
+      <c r="A12" s="138" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="133" t="n">
+      <c r="B12" s="139"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="138" t="n">
         <f aca="false">PRODUCT(C12:D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="133"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="142"/>
-      <c r="K12" s="140"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="147"/>
+      <c r="K12" s="145"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -10859,32 +10945,32 @@
       <c r="AD12" s="0"/>
       <c r="AE12" s="0"/>
       <c r="AF12" s="0"/>
-      <c r="IS12" s="131"/>
+      <c r="IS12" s="136"/>
       <c r="IT12" s="0"/>
       <c r="IU12" s="0"/>
       <c r="IV12" s="0"/>
       <c r="IW12" s="0"/>
       <c r="IX12" s="0"/>
       <c r="IY12" s="0"/>
-      <c r="IZ12" s="144"/>
+      <c r="IZ12" s="149"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="133" t="n">
+      <c r="A13" s="138" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="133" t="n">
+      <c r="B13" s="139"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="138" t="n">
         <f aca="false">PRODUCT(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="133"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="134"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="142"/>
-      <c r="K13" s="140"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="145"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="145"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -10906,22 +10992,22 @@
       <c r="AD13" s="0"/>
       <c r="AE13" s="0"/>
       <c r="AF13" s="0"/>
-      <c r="IS13" s="131"/>
+      <c r="IS13" s="136"/>
       <c r="IT13" s="0"/>
-      <c r="IU13" s="104"/>
-      <c r="IV13" s="104"/>
-      <c r="IW13" s="104"/>
-      <c r="IX13" s="104"/>
-      <c r="IY13" s="104"/>
-      <c r="IZ13" s="145"/>
+      <c r="IU13" s="109"/>
+      <c r="IV13" s="109"/>
+      <c r="IW13" s="109"/>
+      <c r="IX13" s="109"/>
+      <c r="IY13" s="109"/>
+      <c r="IZ13" s="150"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="146"/>
-      <c r="B14" s="146"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="146"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="146"/>
+      <c r="A14" s="151"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="151"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
@@ -10950,12 +11036,12 @@
       <c r="AF14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="146"/>
-      <c r="B15" s="146"/>
-      <c r="C15" s="146"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="146"/>
+      <c r="A15" s="151"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
@@ -10984,12 +11070,12 @@
       <c r="AF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="146"/>
-      <c r="B16" s="146"/>
-      <c r="C16" s="146"/>
-      <c r="D16" s="146"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="146"/>
+      <c r="A16" s="151"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -11018,14 +11104,14 @@
       <c r="AF16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="147" t="s">
-        <v>223</v>
-      </c>
-      <c r="B17" s="147"/>
-      <c r="C17" s="147"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
+      <c r="A17" s="152" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17" s="152"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -11054,18 +11140,18 @@
       <c r="AF17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="B18" s="149" t="s">
-        <v>225</v>
-      </c>
-      <c r="C18" s="148" t="s">
-        <v>226</v>
-      </c>
-      <c r="D18" s="146"/>
-      <c r="E18" s="146"/>
-      <c r="F18" s="146"/>
+      <c r="A18" s="153" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="153" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -11094,18 +11180,18 @@
       <c r="AF18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="148" t="n">
+      <c r="A19" s="153" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="148" t="s">
-        <v>227</v>
-      </c>
-      <c r="C19" s="148" t="s">
-        <v>228</v>
-      </c>
-      <c r="D19" s="150"/>
-      <c r="E19" s="150"/>
-      <c r="F19" s="146"/>
+      <c r="B19" s="153" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="153" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="155"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="151"/>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -11134,14 +11220,14 @@
       <c r="AF19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="151" t="n">
+      <c r="A20" s="156" t="n">
         <v>2</v>
       </c>
-      <c r="B20" s="151" t="s">
-        <v>229</v>
-      </c>
-      <c r="C20" s="151" t="s">
-        <v>230</v>
+      <c r="B20" s="156" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="156" t="s">
+        <v>237</v>
       </c>
       <c r="D20" s="0"/>
       <c r="G20" s="0"/>
@@ -11172,14 +11258,14 @@
       <c r="AF20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="151" t="n">
+      <c r="A21" s="156" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="151" t="s">
-        <v>231</v>
-      </c>
-      <c r="C21" s="151" t="s">
-        <v>232</v>
+      <c r="B21" s="156" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" s="156" t="s">
+        <v>239</v>
       </c>
       <c r="D21" s="0"/>
       <c r="G21" s="0"/>
@@ -11210,14 +11296,14 @@
       <c r="AF21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="151" t="n">
+      <c r="A22" s="156" t="n">
         <v>4</v>
       </c>
-      <c r="B22" s="151" t="s">
-        <v>233</v>
-      </c>
-      <c r="C22" s="151" t="s">
-        <v>234</v>
+      <c r="B22" s="156" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" s="156" t="s">
+        <v>241</v>
       </c>
       <c r="D22" s="0"/>
       <c r="G22" s="0"/>
@@ -11368,184 +11454,184 @@
       <c r="AF26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="146"/>
-      <c r="D27" s="146"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="95"/>
-      <c r="N27" s="95"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="95"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="95"/>
-      <c r="U27" s="95"/>
-      <c r="V27" s="95"/>
-      <c r="W27" s="95"/>
-      <c r="X27" s="95"/>
-      <c r="Y27" s="95"/>
-      <c r="Z27" s="95"/>
-      <c r="AA27" s="95"/>
-      <c r="AB27" s="95"/>
-      <c r="AC27" s="95"/>
-      <c r="AD27" s="95"/>
-      <c r="AE27" s="95"/>
-      <c r="AF27" s="95"/>
+      <c r="C27" s="151"/>
+      <c r="D27" s="151"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="100"/>
+      <c r="R27" s="100"/>
+      <c r="S27" s="100"/>
+      <c r="T27" s="100"/>
+      <c r="U27" s="100"/>
+      <c r="V27" s="100"/>
+      <c r="W27" s="100"/>
+      <c r="X27" s="100"/>
+      <c r="Y27" s="100"/>
+      <c r="Z27" s="100"/>
+      <c r="AA27" s="100"/>
+      <c r="AB27" s="100"/>
+      <c r="AC27" s="100"/>
+      <c r="AD27" s="100"/>
+      <c r="AE27" s="100"/>
+      <c r="AF27" s="100"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="95"/>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="95"/>
-      <c r="S28" s="95"/>
-      <c r="T28" s="95"/>
-      <c r="U28" s="95"/>
-      <c r="V28" s="95"/>
-      <c r="W28" s="95"/>
-      <c r="X28" s="95"/>
-      <c r="Y28" s="95"/>
-      <c r="Z28" s="95"/>
-      <c r="AA28" s="95"/>
-      <c r="AB28" s="95"/>
-      <c r="AC28" s="95"/>
-      <c r="AD28" s="95"/>
-      <c r="AE28" s="95"/>
-      <c r="AF28" s="95"/>
+      <c r="C28" s="151"/>
+      <c r="D28" s="151"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="100"/>
+      <c r="R28" s="100"/>
+      <c r="S28" s="100"/>
+      <c r="T28" s="100"/>
+      <c r="U28" s="100"/>
+      <c r="V28" s="100"/>
+      <c r="W28" s="100"/>
+      <c r="X28" s="100"/>
+      <c r="Y28" s="100"/>
+      <c r="Z28" s="100"/>
+      <c r="AA28" s="100"/>
+      <c r="AB28" s="100"/>
+      <c r="AC28" s="100"/>
+      <c r="AD28" s="100"/>
+      <c r="AE28" s="100"/>
+      <c r="AF28" s="100"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="146"/>
-      <c r="D29" s="146"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="95"/>
-      <c r="I29" s="95"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="95"/>
-      <c r="M29" s="95"/>
-      <c r="N29" s="95"/>
-      <c r="O29" s="95"/>
-      <c r="P29" s="95"/>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="95"/>
-      <c r="S29" s="95"/>
-      <c r="T29" s="95"/>
-      <c r="U29" s="95"/>
-      <c r="V29" s="95"/>
-      <c r="W29" s="95"/>
-      <c r="X29" s="95"/>
-      <c r="Y29" s="95"/>
-      <c r="Z29" s="95"/>
-      <c r="AA29" s="95"/>
-      <c r="AB29" s="95"/>
-      <c r="AC29" s="95"/>
-      <c r="AD29" s="95"/>
-      <c r="AE29" s="95"/>
-      <c r="AF29" s="95"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="151"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="100"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="100"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="100"/>
+      <c r="R29" s="100"/>
+      <c r="S29" s="100"/>
+      <c r="T29" s="100"/>
+      <c r="U29" s="100"/>
+      <c r="V29" s="100"/>
+      <c r="W29" s="100"/>
+      <c r="X29" s="100"/>
+      <c r="Y29" s="100"/>
+      <c r="Z29" s="100"/>
+      <c r="AA29" s="100"/>
+      <c r="AB29" s="100"/>
+      <c r="AC29" s="100"/>
+      <c r="AD29" s="100"/>
+      <c r="AE29" s="100"/>
+      <c r="AF29" s="100"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="152"/>
-      <c r="D30" s="152"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="95"/>
-      <c r="M30" s="95"/>
-      <c r="N30" s="95"/>
-      <c r="O30" s="95"/>
-      <c r="P30" s="95"/>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="95"/>
-      <c r="S30" s="95"/>
-      <c r="T30" s="95"/>
-      <c r="U30" s="95"/>
-      <c r="V30" s="95"/>
-      <c r="W30" s="95"/>
-      <c r="X30" s="95"/>
-      <c r="Y30" s="95"/>
-      <c r="Z30" s="95"/>
-      <c r="AA30" s="95"/>
-      <c r="AB30" s="95"/>
-      <c r="AC30" s="95"/>
-      <c r="AD30" s="95"/>
-      <c r="AE30" s="95"/>
-      <c r="AF30" s="95"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="100"/>
+      <c r="R30" s="100"/>
+      <c r="S30" s="100"/>
+      <c r="T30" s="100"/>
+      <c r="U30" s="100"/>
+      <c r="V30" s="100"/>
+      <c r="W30" s="100"/>
+      <c r="X30" s="100"/>
+      <c r="Y30" s="100"/>
+      <c r="Z30" s="100"/>
+      <c r="AA30" s="100"/>
+      <c r="AB30" s="100"/>
+      <c r="AC30" s="100"/>
+      <c r="AD30" s="100"/>
+      <c r="AE30" s="100"/>
+      <c r="AF30" s="100"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="152"/>
-      <c r="D31" s="152"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="95"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="95"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="95"/>
-      <c r="R31" s="95"/>
-      <c r="S31" s="95"/>
-      <c r="T31" s="95"/>
-      <c r="U31" s="95"/>
-      <c r="V31" s="95"/>
-      <c r="W31" s="95"/>
-      <c r="X31" s="95"/>
-      <c r="Y31" s="95"/>
-      <c r="Z31" s="95"/>
-      <c r="AA31" s="95"/>
-      <c r="AB31" s="95"/>
-      <c r="AC31" s="95"/>
-      <c r="AD31" s="95"/>
-      <c r="AE31" s="95"/>
-      <c r="AF31" s="95"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="100"/>
+      <c r="S31" s="100"/>
+      <c r="T31" s="100"/>
+      <c r="U31" s="100"/>
+      <c r="V31" s="100"/>
+      <c r="W31" s="100"/>
+      <c r="X31" s="100"/>
+      <c r="Y31" s="100"/>
+      <c r="Z31" s="100"/>
+      <c r="AA31" s="100"/>
+      <c r="AB31" s="100"/>
+      <c r="AC31" s="100"/>
+      <c r="AD31" s="100"/>
+      <c r="AE31" s="100"/>
+      <c r="AF31" s="100"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="152"/>
-      <c r="D32" s="152"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
-      <c r="K32" s="95"/>
-      <c r="L32" s="95"/>
-      <c r="M32" s="95"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="95"/>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="95"/>
-      <c r="S32" s="95"/>
-      <c r="T32" s="95"/>
-      <c r="U32" s="95"/>
-      <c r="V32" s="95"/>
-      <c r="W32" s="95"/>
-      <c r="X32" s="95"/>
-      <c r="Y32" s="95"/>
-      <c r="Z32" s="95"/>
-      <c r="AA32" s="95"/>
-      <c r="AB32" s="95"/>
-      <c r="AC32" s="95"/>
-      <c r="AD32" s="95"/>
-      <c r="AE32" s="95"/>
-      <c r="AF32" s="95"/>
+      <c r="C32" s="157"/>
+      <c r="D32" s="157"/>
+      <c r="G32" s="100"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="100"/>
+      <c r="Q32" s="100"/>
+      <c r="R32" s="100"/>
+      <c r="S32" s="100"/>
+      <c r="T32" s="100"/>
+      <c r="U32" s="100"/>
+      <c r="V32" s="100"/>
+      <c r="W32" s="100"/>
+      <c r="X32" s="100"/>
+      <c r="Y32" s="100"/>
+      <c r="Z32" s="100"/>
+      <c r="AA32" s="100"/>
+      <c r="AB32" s="100"/>
+      <c r="AC32" s="100"/>
+      <c r="AD32" s="100"/>
+      <c r="AE32" s="100"/>
+      <c r="AF32" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Actualizacion mensual del plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
+++ b/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -58,6 +58,7 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Sheet_Title" vbProcedure="false">"Plan Riesgos"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
@@ -166,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="268">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -794,6 +795,9 @@
   </si>
   <si>
     <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Los recursos descritos abajo son de tipo muy general, esto se puede apreciar mas especificamente en el archivo inventario de equipos y cuentas de colaboradores de la carpeta documentos adicionales /referencias en la raíz de las carpetas</t>
   </si>
   <si>
     <t>Internet</t>
@@ -1494,7 +1498,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1900,6 +1904,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2360,7 +2368,7 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -10309,10 +10317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10370,161 +10378,173 @@
       </c>
       <c r="I3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="42.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="I4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="103" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="B5" s="104" t="s">
         <v>207</v>
       </c>
-      <c r="D4" s="104" t="n">
+      <c r="C5" s="104" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="105" t="n">
         <v>42380</v>
       </c>
-      <c r="E4" s="104" t="n">
+      <c r="E5" s="105" t="n">
         <v>42373</v>
       </c>
-      <c r="F4" s="103"/>
-      <c r="I4" s="105"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="102" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="103" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="103" t="s">
+      <c r="F5" s="104"/>
+      <c r="I5" s="106"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="103" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="104" t="n">
+      <c r="B6" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="104" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="105" t="n">
         <v>42380</v>
       </c>
-      <c r="E5" s="104" t="n">
+      <c r="E6" s="105" t="n">
         <v>42373</v>
       </c>
-      <c r="F5" s="103"/>
-      <c r="I5" s="105"/>
-    </row>
-    <row r="6" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="102" t="s">
+      <c r="F6" s="104"/>
+      <c r="I6" s="106"/>
+    </row>
+    <row r="7" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="104" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="104" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="105" t="n">
+        <v>42380</v>
+      </c>
+      <c r="E7" s="105" t="n">
+        <v>42373</v>
+      </c>
+      <c r="F7" s="104" t="s">
+        <v>214</v>
+      </c>
+      <c r="I7" s="106"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="103" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="104" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="103" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="103" t="s">
-        <v>212</v>
-      </c>
-      <c r="D6" s="104" t="n">
+      <c r="D8" s="105" t="n">
         <v>42380</v>
       </c>
-      <c r="E6" s="104" t="n">
+      <c r="E8" s="105" t="n">
         <v>42373</v>
       </c>
-      <c r="F6" s="103" t="s">
-        <v>213</v>
-      </c>
-      <c r="I6" s="105"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="102" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" s="103" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="103" t="s">
-        <v>209</v>
-      </c>
-      <c r="D7" s="104" t="n">
+      <c r="F8" s="104"/>
+      <c r="I8" s="106"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="103" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="105" t="n">
         <v>42380</v>
       </c>
-      <c r="E7" s="104" t="n">
+      <c r="E9" s="105" t="n">
         <v>42373</v>
       </c>
-      <c r="F7" s="103"/>
-      <c r="I7" s="105"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="102" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" s="103" t="s">
-        <v>206</v>
-      </c>
-      <c r="C8" s="103" t="s">
-        <v>209</v>
-      </c>
-      <c r="D8" s="104" t="n">
-        <v>42380</v>
-      </c>
-      <c r="E8" s="104" t="n">
-        <v>42373</v>
-      </c>
-      <c r="F8" s="103"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="106"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="103"/>
+      <c r="F9" s="104"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="102"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="103"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="104"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="102"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="103"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="104"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="102"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="103"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="104"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="103"/>
-      <c r="B13" s="103"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="104"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="103"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="103"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.611111111111111" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -10565,10 +10585,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="109"/>
+      <c r="A1" s="110"/>
       <c r="B1" s="0"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -10609,19 +10629,19 @@
       <c r="JA1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="111" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
+      <c r="A2" s="112" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
@@ -10643,31 +10663,31 @@
       <c r="AD2" s="0"/>
       <c r="AE2" s="0"/>
       <c r="AF2" s="0"/>
-      <c r="IR2" s="112" t="s">
-        <v>217</v>
-      </c>
-      <c r="IS2" s="112"/>
-      <c r="IT2" s="112"/>
-      <c r="IU2" s="112"/>
-      <c r="IV2" s="112"/>
-      <c r="IW2" s="112"/>
-      <c r="IX2" s="112"/>
-      <c r="IY2" s="112"/>
-      <c r="IZ2" s="112"/>
-      <c r="JA2" s="112"/>
+      <c r="IR2" s="113" t="s">
+        <v>218</v>
+      </c>
+      <c r="IS2" s="113"/>
+      <c r="IT2" s="113"/>
+      <c r="IU2" s="113"/>
+      <c r="IV2" s="113"/>
+      <c r="IW2" s="113"/>
+      <c r="IX2" s="113"/>
+      <c r="IY2" s="113"/>
+      <c r="IZ2" s="113"/>
+      <c r="JA2" s="113"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="111"/>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
@@ -10687,11 +10707,11 @@
       <c r="AB3" s="0"/>
       <c r="AC3" s="0"/>
       <c r="AD3" s="0"/>
-      <c r="AE3" s="113" t="s">
-        <v>218</v>
-      </c>
-      <c r="AF3" s="113" t="s">
+      <c r="AE3" s="114" t="s">
         <v>219</v>
+      </c>
+      <c r="AF3" s="114" t="s">
+        <v>220</v>
       </c>
       <c r="IS3" s="0"/>
       <c r="IT3" s="0"/>
@@ -10703,38 +10723,38 @@
       <c r="IZ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="114" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" s="115" t="s">
+      <c r="A4" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="C4" s="116" t="s">
+      <c r="B4" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="C4" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="E4" s="116" t="s">
+      <c r="D4" s="117" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="116" t="s">
+      <c r="E4" s="117" t="s">
         <v>225</v>
       </c>
-      <c r="G4" s="116" t="s">
+      <c r="F4" s="117" t="s">
         <v>226</v>
       </c>
-      <c r="H4" s="116" t="s">
+      <c r="G4" s="117" t="s">
         <v>227</v>
       </c>
-      <c r="I4" s="116" t="s">
+      <c r="H4" s="117" t="s">
         <v>228</v>
       </c>
-      <c r="J4" s="117" t="s">
+      <c r="I4" s="117" t="s">
         <v>229</v>
       </c>
-      <c r="K4" s="116" t="s">
+      <c r="J4" s="118" t="s">
         <v>230</v>
+      </c>
+      <c r="K4" s="117" t="s">
+        <v>231</v>
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -10755,11 +10775,11 @@
       <c r="AB4" s="0"/>
       <c r="AC4" s="0"/>
       <c r="AD4" s="0"/>
-      <c r="AE4" s="118" t="s">
-        <v>218</v>
-      </c>
-      <c r="AF4" s="118" t="s">
+      <c r="AE4" s="119" t="s">
         <v>219</v>
+      </c>
+      <c r="AF4" s="119" t="s">
+        <v>220</v>
       </c>
       <c r="IS4" s="0"/>
       <c r="IT4" s="0"/>
@@ -10771,39 +10791,39 @@
       <c r="IZ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="54.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="119" t="n">
+      <c r="A5" s="120" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="120" t="s">
-        <v>231</v>
-      </c>
-      <c r="C5" s="119" t="n">
+      <c r="B5" s="121" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="120" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="121" t="n">
+      <c r="D5" s="122" t="n">
         <v>0.3</v>
       </c>
-      <c r="E5" s="119" t="n">
+      <c r="E5" s="120" t="n">
         <f aca="false">PRODUCT(A5:D5)</f>
         <v>1.5</v>
       </c>
-      <c r="F5" s="119" t="n">
+      <c r="F5" s="120" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="H5" s="120" t="s">
+      <c r="G5" s="121" t="s">
         <v>233</v>
       </c>
-      <c r="I5" s="119" t="s">
+      <c r="H5" s="121" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="120" t="s">
         <v>157</v>
       </c>
-      <c r="J5" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="K5" s="123" t="s">
+      <c r="J5" s="123" t="s">
         <v>235</v>
+      </c>
+      <c r="K5" s="124" t="s">
+        <v>236</v>
       </c>
       <c r="L5" s="0"/>
       <c r="M5" s="0"/>
@@ -10826,70 +10846,70 @@
       <c r="AD5" s="0"/>
       <c r="AE5" s="0"/>
       <c r="AF5" s="0"/>
-      <c r="IS5" s="124" t="s">
-        <v>236</v>
-      </c>
-      <c r="IT5" s="125" t="s">
+      <c r="IS5" s="125" t="s">
         <v>237</v>
       </c>
-      <c r="IU5" s="126" t="n">
+      <c r="IT5" s="126" t="s">
+        <v>238</v>
+      </c>
+      <c r="IU5" s="127" t="n">
         <v>0.9</v>
       </c>
-      <c r="IV5" s="127" t="n">
+      <c r="IV5" s="128" t="n">
         <f aca="false">(IV9*IU5)</f>
         <v>0.9</v>
       </c>
-      <c r="IW5" s="128" t="n">
+      <c r="IW5" s="129" t="n">
         <f aca="false">(IW9*IU5)</f>
         <v>1.8</v>
       </c>
-      <c r="IX5" s="129" t="n">
+      <c r="IX5" s="130" t="n">
         <f aca="false">(IX9*IU5)</f>
         <v>2.7</v>
       </c>
-      <c r="IY5" s="130" t="n">
+      <c r="IY5" s="131" t="n">
         <f aca="false">(IY9*IU5)</f>
         <v>3.6</v>
       </c>
-      <c r="IZ5" s="131" t="n">
+      <c r="IZ5" s="132" t="n">
         <f aca="false">(IZ9*IU5)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="119" t="n">
+      <c r="A6" s="120" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="120" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="119" t="n">
+      <c r="B6" s="121" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="120" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="121" t="n">
+      <c r="D6" s="122" t="n">
         <v>0.2</v>
       </c>
-      <c r="E6" s="119" t="n">
+      <c r="E6" s="120" t="n">
         <f aca="false">PRODUCT(C6:D6)</f>
         <v>0.8</v>
       </c>
-      <c r="F6" s="119" t="n">
+      <c r="F6" s="120" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="120" t="s">
-        <v>239</v>
-      </c>
-      <c r="H6" s="120" t="s">
+      <c r="G6" s="121" t="s">
         <v>240</v>
       </c>
-      <c r="I6" s="119" t="s">
+      <c r="H6" s="121" t="s">
+        <v>241</v>
+      </c>
+      <c r="I6" s="120" t="s">
         <v>157</v>
       </c>
-      <c r="J6" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="K6" s="123" t="s">
+      <c r="J6" s="123" t="s">
         <v>235</v>
+      </c>
+      <c r="K6" s="124" t="s">
+        <v>236</v>
       </c>
       <c r="L6" s="0"/>
       <c r="M6" s="0"/>
@@ -10912,68 +10932,68 @@
       <c r="AD6" s="0"/>
       <c r="AE6" s="0"/>
       <c r="AF6" s="0"/>
-      <c r="IS6" s="124"/>
-      <c r="IT6" s="125" t="s">
-        <v>241</v>
-      </c>
-      <c r="IU6" s="126" t="n">
+      <c r="IS6" s="125"/>
+      <c r="IT6" s="126" t="s">
+        <v>242</v>
+      </c>
+      <c r="IU6" s="127" t="n">
         <v>0.5</v>
       </c>
-      <c r="IV6" s="132" t="n">
+      <c r="IV6" s="133" t="n">
         <f aca="false">(IV9*IU6)</f>
         <v>0.5</v>
       </c>
-      <c r="IW6" s="133" t="n">
+      <c r="IW6" s="134" t="n">
         <f aca="false">(IW9*IU6)</f>
         <v>1</v>
       </c>
-      <c r="IX6" s="134" t="n">
+      <c r="IX6" s="135" t="n">
         <f aca="false">(IX9*IU6)</f>
         <v>1.5</v>
       </c>
-      <c r="IY6" s="134" t="n">
+      <c r="IY6" s="135" t="n">
         <f aca="false">(IY9*IU6)</f>
         <v>2</v>
       </c>
-      <c r="IZ6" s="135" t="n">
+      <c r="IZ6" s="136" t="n">
         <f aca="false">(IZ9*IU6)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="119" t="n">
+      <c r="A7" s="120" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="120" t="s">
-        <v>242</v>
-      </c>
-      <c r="C7" s="119" t="n">
+      <c r="B7" s="121" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="120" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="121" t="n">
+      <c r="D7" s="122" t="n">
         <v>0.01</v>
       </c>
-      <c r="E7" s="119" t="n">
+      <c r="E7" s="120" t="n">
         <f aca="false">PRODUCT(C7:D7)</f>
         <v>0.05</v>
       </c>
-      <c r="F7" s="119" t="n">
+      <c r="F7" s="120" t="n">
         <v>4</v>
       </c>
-      <c r="G7" s="120" t="s">
-        <v>243</v>
-      </c>
-      <c r="H7" s="120" t="s">
+      <c r="G7" s="121" t="s">
         <v>244</v>
       </c>
-      <c r="I7" s="119" t="s">
+      <c r="H7" s="121" t="s">
+        <v>245</v>
+      </c>
+      <c r="I7" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="K7" s="123" t="s">
+      <c r="J7" s="123" t="s">
         <v>235</v>
+      </c>
+      <c r="K7" s="124" t="s">
+        <v>236</v>
       </c>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -10996,68 +11016,68 @@
       <c r="AD7" s="0"/>
       <c r="AE7" s="0"/>
       <c r="AF7" s="0"/>
-      <c r="IS7" s="124"/>
-      <c r="IT7" s="125" t="s">
-        <v>245</v>
-      </c>
-      <c r="IU7" s="126" t="n">
+      <c r="IS7" s="125"/>
+      <c r="IT7" s="126" t="s">
+        <v>246</v>
+      </c>
+      <c r="IU7" s="127" t="n">
         <v>0.3</v>
       </c>
-      <c r="IV7" s="136" t="n">
+      <c r="IV7" s="137" t="n">
         <f aca="false">(IV9*IU7)</f>
         <v>0.3</v>
       </c>
-      <c r="IW7" s="137" t="n">
+      <c r="IW7" s="138" t="n">
         <f aca="false">(IW9*IU7)</f>
         <v>0.6</v>
       </c>
-      <c r="IX7" s="134" t="n">
+      <c r="IX7" s="135" t="n">
         <f aca="false">(IX9*IU7)</f>
         <v>0.9</v>
       </c>
-      <c r="IY7" s="134" t="n">
+      <c r="IY7" s="135" t="n">
         <f aca="false">(IY9*IU7)</f>
         <v>1.2</v>
       </c>
-      <c r="IZ7" s="138" t="n">
+      <c r="IZ7" s="139" t="n">
         <f aca="false">(IZ9*IU7)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="119" t="n">
+      <c r="A8" s="120" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="120" t="s">
-        <v>246</v>
-      </c>
-      <c r="C8" s="119" t="n">
+      <c r="B8" s="121" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" s="120" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="121" t="n">
+      <c r="D8" s="122" t="n">
         <v>0.4</v>
       </c>
-      <c r="E8" s="119" t="n">
+      <c r="E8" s="120" t="n">
         <f aca="false">PRODUCT(C8:D8)</f>
         <v>2</v>
       </c>
-      <c r="F8" s="119" t="n">
+      <c r="F8" s="120" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="120" t="s">
-        <v>247</v>
-      </c>
-      <c r="H8" s="120" t="s">
+      <c r="G8" s="121" t="s">
         <v>248</v>
       </c>
-      <c r="I8" s="119" t="s">
+      <c r="H8" s="121" t="s">
+        <v>249</v>
+      </c>
+      <c r="I8" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="K8" s="123" t="s">
+      <c r="J8" s="123" t="s">
         <v>235</v>
+      </c>
+      <c r="K8" s="124" t="s">
+        <v>236</v>
       </c>
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
@@ -11080,68 +11100,68 @@
       <c r="AD8" s="0"/>
       <c r="AE8" s="0"/>
       <c r="AF8" s="0"/>
-      <c r="IS8" s="124"/>
-      <c r="IT8" s="125" t="s">
-        <v>241</v>
-      </c>
-      <c r="IU8" s="139" t="n">
+      <c r="IS8" s="125"/>
+      <c r="IT8" s="126" t="s">
+        <v>242</v>
+      </c>
+      <c r="IU8" s="140" t="n">
         <v>0.1</v>
       </c>
-      <c r="IV8" s="140" t="n">
+      <c r="IV8" s="141" t="n">
         <f aca="false">(IV9*IU8)</f>
         <v>0.1</v>
       </c>
-      <c r="IW8" s="141" t="n">
+      <c r="IW8" s="142" t="n">
         <f aca="false">(IW9*IU8)</f>
         <v>0.2</v>
       </c>
-      <c r="IX8" s="142" t="n">
+      <c r="IX8" s="143" t="n">
         <f aca="false">(IX9*IV8)</f>
         <v>0.3</v>
       </c>
-      <c r="IY8" s="142" t="n">
+      <c r="IY8" s="143" t="n">
         <f aca="false">(IY9*IU8)</f>
         <v>0.4</v>
       </c>
-      <c r="IZ8" s="143" t="n">
+      <c r="IZ8" s="144" t="n">
         <f aca="false">(IZ9*IU8)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="144" t="n">
+      <c r="A9" s="145" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="120" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" s="119" t="n">
+      <c r="B9" s="121" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="120" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="121" t="n">
+      <c r="D9" s="122" t="n">
         <v>0.2</v>
       </c>
-      <c r="E9" s="119" t="n">
+      <c r="E9" s="120" t="n">
         <f aca="false">PRODUCT(C9:D9)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="119" t="n">
+      <c r="F9" s="120" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="120" t="s">
-        <v>250</v>
-      </c>
-      <c r="H9" s="120" t="s">
+      <c r="G9" s="121" t="s">
         <v>251</v>
       </c>
-      <c r="I9" s="119" t="s">
+      <c r="H9" s="121" t="s">
+        <v>252</v>
+      </c>
+      <c r="I9" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="K9" s="123" t="s">
+      <c r="J9" s="123" t="s">
         <v>235</v>
+      </c>
+      <c r="K9" s="124" t="s">
+        <v>236</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
@@ -11164,59 +11184,59 @@
       <c r="AD9" s="0"/>
       <c r="AE9" s="0"/>
       <c r="AF9" s="0"/>
-      <c r="IS9" s="145"/>
+      <c r="IS9" s="146"/>
       <c r="IT9" s="0"/>
-      <c r="IU9" s="125"/>
-      <c r="IV9" s="126" t="n">
+      <c r="IU9" s="126"/>
+      <c r="IV9" s="127" t="n">
         <v>1</v>
       </c>
-      <c r="IW9" s="126" t="n">
+      <c r="IW9" s="127" t="n">
         <v>2</v>
       </c>
-      <c r="IX9" s="126" t="n">
+      <c r="IX9" s="127" t="n">
         <v>3</v>
       </c>
-      <c r="IY9" s="126" t="n">
+      <c r="IY9" s="127" t="n">
         <v>4</v>
       </c>
-      <c r="IZ9" s="146" t="n">
+      <c r="IZ9" s="147" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="147" t="n">
+      <c r="A10" s="148" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="148" t="s">
-        <v>252</v>
-      </c>
-      <c r="C10" s="119" t="n">
+      <c r="B10" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="120" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="121" t="n">
+      <c r="D10" s="122" t="n">
         <v>0.2</v>
       </c>
-      <c r="E10" s="119" t="n">
+      <c r="E10" s="120" t="n">
         <f aca="false">PRODUCT(C10:D10)</f>
         <v>1</v>
       </c>
-      <c r="F10" s="119" t="n">
+      <c r="F10" s="120" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="149" t="s">
-        <v>253</v>
-      </c>
-      <c r="H10" s="150" t="s">
+      <c r="G10" s="150" t="s">
         <v>254</v>
       </c>
-      <c r="I10" s="119" t="s">
+      <c r="H10" s="151" t="s">
+        <v>255</v>
+      </c>
+      <c r="I10" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="K10" s="151" t="s">
+      <c r="J10" s="123" t="s">
         <v>235</v>
+      </c>
+      <c r="K10" s="152" t="s">
+        <v>236</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
@@ -11239,42 +11259,42 @@
       <c r="AD10" s="0"/>
       <c r="AE10" s="0"/>
       <c r="AF10" s="0"/>
-      <c r="IS10" s="145"/>
+      <c r="IS10" s="146"/>
       <c r="IT10" s="0"/>
       <c r="IU10" s="0"/>
-      <c r="IV10" s="125" t="s">
-        <v>241</v>
-      </c>
-      <c r="IW10" s="125" t="s">
-        <v>245</v>
-      </c>
-      <c r="IX10" s="125" t="s">
-        <v>255</v>
-      </c>
-      <c r="IY10" s="125" t="s">
+      <c r="IV10" s="126" t="s">
+        <v>242</v>
+      </c>
+      <c r="IW10" s="126" t="s">
+        <v>246</v>
+      </c>
+      <c r="IX10" s="126" t="s">
         <v>256</v>
       </c>
-      <c r="IZ10" s="152" t="s">
-        <v>237</v>
+      <c r="IY10" s="126" t="s">
+        <v>257</v>
+      </c>
+      <c r="IZ10" s="153" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="147" t="n">
+      <c r="A11" s="148" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="148"/>
-      <c r="C11" s="147"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="147" t="n">
+      <c r="B11" s="149"/>
+      <c r="C11" s="148"/>
+      <c r="D11" s="154"/>
+      <c r="E11" s="148" t="n">
         <f aca="false">PRODUCT(C11:D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="147"/>
-      <c r="G11" s="154"/>
-      <c r="H11" s="148"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="156"/>
-      <c r="K11" s="154"/>
+      <c r="F11" s="148"/>
+      <c r="G11" s="155"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="157"/>
+      <c r="K11" s="155"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
@@ -11296,34 +11316,34 @@
       <c r="AD11" s="0"/>
       <c r="AE11" s="0"/>
       <c r="AF11" s="0"/>
-      <c r="IS11" s="145"/>
+      <c r="IS11" s="146"/>
       <c r="IT11" s="0"/>
-      <c r="IU11" s="126"/>
-      <c r="IV11" s="157" t="s">
-        <v>257</v>
-      </c>
-      <c r="IW11" s="157"/>
-      <c r="IX11" s="157"/>
-      <c r="IY11" s="157"/>
-      <c r="IZ11" s="157"/>
+      <c r="IU11" s="127"/>
+      <c r="IV11" s="158" t="s">
+        <v>258</v>
+      </c>
+      <c r="IW11" s="158"/>
+      <c r="IX11" s="158"/>
+      <c r="IY11" s="158"/>
+      <c r="IZ11" s="158"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="147" t="n">
+      <c r="A12" s="148" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="148"/>
-      <c r="C12" s="147"/>
-      <c r="D12" s="153"/>
-      <c r="E12" s="147" t="n">
+      <c r="B12" s="149"/>
+      <c r="C12" s="148"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="148" t="n">
         <f aca="false">PRODUCT(C12:D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="147"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="155"/>
-      <c r="J12" s="156"/>
-      <c r="K12" s="154"/>
+      <c r="F12" s="148"/>
+      <c r="G12" s="155"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="157"/>
+      <c r="K12" s="155"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -11345,32 +11365,32 @@
       <c r="AD12" s="0"/>
       <c r="AE12" s="0"/>
       <c r="AF12" s="0"/>
-      <c r="IS12" s="145"/>
+      <c r="IS12" s="146"/>
       <c r="IT12" s="0"/>
       <c r="IU12" s="0"/>
       <c r="IV12" s="0"/>
       <c r="IW12" s="0"/>
       <c r="IX12" s="0"/>
       <c r="IY12" s="0"/>
-      <c r="IZ12" s="158"/>
+      <c r="IZ12" s="159"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="147" t="n">
+      <c r="A13" s="148" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="148"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="153"/>
-      <c r="E13" s="147" t="n">
+      <c r="B13" s="149"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="148" t="n">
         <f aca="false">PRODUCT(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="147"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="148"/>
-      <c r="I13" s="155"/>
-      <c r="J13" s="156"/>
-      <c r="K13" s="154"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="156"/>
+      <c r="J13" s="157"/>
+      <c r="K13" s="155"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -11392,22 +11412,22 @@
       <c r="AD13" s="0"/>
       <c r="AE13" s="0"/>
       <c r="AF13" s="0"/>
-      <c r="IS13" s="145"/>
+      <c r="IS13" s="146"/>
       <c r="IT13" s="0"/>
-      <c r="IU13" s="118"/>
-      <c r="IV13" s="118"/>
-      <c r="IW13" s="118"/>
-      <c r="IX13" s="118"/>
-      <c r="IY13" s="118"/>
-      <c r="IZ13" s="159"/>
+      <c r="IU13" s="119"/>
+      <c r="IV13" s="119"/>
+      <c r="IW13" s="119"/>
+      <c r="IX13" s="119"/>
+      <c r="IY13" s="119"/>
+      <c r="IZ13" s="160"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="160"/>
-      <c r="B14" s="160"/>
-      <c r="C14" s="160"/>
-      <c r="D14" s="160"/>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
+      <c r="A14" s="161"/>
+      <c r="B14" s="161"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="161"/>
+      <c r="E14" s="161"/>
+      <c r="F14" s="161"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
@@ -11436,12 +11456,12 @@
       <c r="AF14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="160"/>
-      <c r="B15" s="160"/>
-      <c r="C15" s="160"/>
-      <c r="D15" s="160"/>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
+      <c r="A15" s="161"/>
+      <c r="B15" s="161"/>
+      <c r="C15" s="161"/>
+      <c r="D15" s="161"/>
+      <c r="E15" s="161"/>
+      <c r="F15" s="161"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
@@ -11470,12 +11490,12 @@
       <c r="AF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="160"/>
-      <c r="B16" s="160"/>
-      <c r="C16" s="160"/>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
+      <c r="A16" s="161"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="161"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -11504,14 +11524,14 @@
       <c r="AF16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="161" t="s">
-        <v>258</v>
-      </c>
-      <c r="B17" s="161"/>
-      <c r="C17" s="161"/>
-      <c r="D17" s="160"/>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
+      <c r="A17" s="162" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="162"/>
+      <c r="C17" s="162"/>
+      <c r="D17" s="161"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -11540,18 +11560,18 @@
       <c r="AF17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="162" t="s">
-        <v>259</v>
-      </c>
-      <c r="B18" s="163" t="s">
+      <c r="A18" s="163" t="s">
         <v>260</v>
       </c>
-      <c r="C18" s="162" t="s">
+      <c r="B18" s="164" t="s">
         <v>261</v>
       </c>
-      <c r="D18" s="160"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
+      <c r="C18" s="163" t="s">
+        <v>262</v>
+      </c>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -11580,18 +11600,18 @@
       <c r="AF18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="162" t="n">
+      <c r="A19" s="163" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="162" t="s">
-        <v>262</v>
-      </c>
-      <c r="C19" s="162" t="s">
+      <c r="B19" s="163" t="s">
         <v>263</v>
       </c>
-      <c r="D19" s="164"/>
-      <c r="E19" s="164"/>
-      <c r="F19" s="160"/>
+      <c r="C19" s="163" t="s">
+        <v>264</v>
+      </c>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="161"/>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -11620,13 +11640,13 @@
       <c r="AF19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="165" t="n">
+      <c r="A20" s="166" t="n">
         <v>2</v>
       </c>
-      <c r="B20" s="165" t="s">
-        <v>264</v>
-      </c>
-      <c r="C20" s="165" t="s">
+      <c r="B20" s="166" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" s="166" t="s">
         <v>134</v>
       </c>
       <c r="D20" s="0"/>
@@ -11658,13 +11678,13 @@
       <c r="AF20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="165" t="n">
+      <c r="A21" s="166" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="165" t="s">
-        <v>265</v>
-      </c>
-      <c r="C21" s="165" t="s">
+      <c r="B21" s="166" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" s="166" t="s">
         <v>133</v>
       </c>
       <c r="D21" s="0"/>
@@ -11696,13 +11716,13 @@
       <c r="AF21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="165" t="n">
+      <c r="A22" s="166" t="n">
         <v>4</v>
       </c>
-      <c r="B22" s="165" t="s">
-        <v>266</v>
-      </c>
-      <c r="C22" s="165" t="s">
+      <c r="B22" s="166" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22" s="166" t="s">
         <v>132</v>
       </c>
       <c r="D22" s="0"/>
@@ -11854,184 +11874,184 @@
       <c r="AF26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="160"/>
-      <c r="D27" s="160"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="109"/>
-      <c r="P27" s="109"/>
-      <c r="Q27" s="109"/>
-      <c r="R27" s="109"/>
-      <c r="S27" s="109"/>
-      <c r="T27" s="109"/>
-      <c r="U27" s="109"/>
-      <c r="V27" s="109"/>
-      <c r="W27" s="109"/>
-      <c r="X27" s="109"/>
-      <c r="Y27" s="109"/>
-      <c r="Z27" s="109"/>
-      <c r="AA27" s="109"/>
-      <c r="AB27" s="109"/>
-      <c r="AC27" s="109"/>
-      <c r="AD27" s="109"/>
-      <c r="AE27" s="109"/>
-      <c r="AF27" s="109"/>
+      <c r="C27" s="161"/>
+      <c r="D27" s="161"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="110"/>
+      <c r="N27" s="110"/>
+      <c r="O27" s="110"/>
+      <c r="P27" s="110"/>
+      <c r="Q27" s="110"/>
+      <c r="R27" s="110"/>
+      <c r="S27" s="110"/>
+      <c r="T27" s="110"/>
+      <c r="U27" s="110"/>
+      <c r="V27" s="110"/>
+      <c r="W27" s="110"/>
+      <c r="X27" s="110"/>
+      <c r="Y27" s="110"/>
+      <c r="Z27" s="110"/>
+      <c r="AA27" s="110"/>
+      <c r="AB27" s="110"/>
+      <c r="AC27" s="110"/>
+      <c r="AD27" s="110"/>
+      <c r="AE27" s="110"/>
+      <c r="AF27" s="110"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="109"/>
-      <c r="J28" s="109"/>
-      <c r="K28" s="109"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="109"/>
-      <c r="N28" s="109"/>
-      <c r="O28" s="109"/>
-      <c r="P28" s="109"/>
-      <c r="Q28" s="109"/>
-      <c r="R28" s="109"/>
-      <c r="S28" s="109"/>
-      <c r="T28" s="109"/>
-      <c r="U28" s="109"/>
-      <c r="V28" s="109"/>
-      <c r="W28" s="109"/>
-      <c r="X28" s="109"/>
-      <c r="Y28" s="109"/>
-      <c r="Z28" s="109"/>
-      <c r="AA28" s="109"/>
-      <c r="AB28" s="109"/>
-      <c r="AC28" s="109"/>
-      <c r="AD28" s="109"/>
-      <c r="AE28" s="109"/>
-      <c r="AF28" s="109"/>
+      <c r="C28" s="161"/>
+      <c r="D28" s="161"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="110"/>
+      <c r="L28" s="110"/>
+      <c r="M28" s="110"/>
+      <c r="N28" s="110"/>
+      <c r="O28" s="110"/>
+      <c r="P28" s="110"/>
+      <c r="Q28" s="110"/>
+      <c r="R28" s="110"/>
+      <c r="S28" s="110"/>
+      <c r="T28" s="110"/>
+      <c r="U28" s="110"/>
+      <c r="V28" s="110"/>
+      <c r="W28" s="110"/>
+      <c r="X28" s="110"/>
+      <c r="Y28" s="110"/>
+      <c r="Z28" s="110"/>
+      <c r="AA28" s="110"/>
+      <c r="AB28" s="110"/>
+      <c r="AC28" s="110"/>
+      <c r="AD28" s="110"/>
+      <c r="AE28" s="110"/>
+      <c r="AF28" s="110"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="160"/>
-      <c r="D29" s="160"/>
-      <c r="G29" s="109"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="109"/>
-      <c r="J29" s="109"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="109"/>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="109"/>
-      <c r="P29" s="109"/>
-      <c r="Q29" s="109"/>
-      <c r="R29" s="109"/>
-      <c r="S29" s="109"/>
-      <c r="T29" s="109"/>
-      <c r="U29" s="109"/>
-      <c r="V29" s="109"/>
-      <c r="W29" s="109"/>
-      <c r="X29" s="109"/>
-      <c r="Y29" s="109"/>
-      <c r="Z29" s="109"/>
-      <c r="AA29" s="109"/>
-      <c r="AB29" s="109"/>
-      <c r="AC29" s="109"/>
-      <c r="AD29" s="109"/>
-      <c r="AE29" s="109"/>
-      <c r="AF29" s="109"/>
+      <c r="C29" s="161"/>
+      <c r="D29" s="161"/>
+      <c r="G29" s="110"/>
+      <c r="H29" s="110"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="110"/>
+      <c r="L29" s="110"/>
+      <c r="M29" s="110"/>
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
+      <c r="R29" s="110"/>
+      <c r="S29" s="110"/>
+      <c r="T29" s="110"/>
+      <c r="U29" s="110"/>
+      <c r="V29" s="110"/>
+      <c r="W29" s="110"/>
+      <c r="X29" s="110"/>
+      <c r="Y29" s="110"/>
+      <c r="Z29" s="110"/>
+      <c r="AA29" s="110"/>
+      <c r="AB29" s="110"/>
+      <c r="AC29" s="110"/>
+      <c r="AD29" s="110"/>
+      <c r="AE29" s="110"/>
+      <c r="AF29" s="110"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="166"/>
-      <c r="D30" s="166"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="109"/>
-      <c r="J30" s="109"/>
-      <c r="K30" s="109"/>
-      <c r="L30" s="109"/>
-      <c r="M30" s="109"/>
-      <c r="N30" s="109"/>
-      <c r="O30" s="109"/>
-      <c r="P30" s="109"/>
-      <c r="Q30" s="109"/>
-      <c r="R30" s="109"/>
-      <c r="S30" s="109"/>
-      <c r="T30" s="109"/>
-      <c r="U30" s="109"/>
-      <c r="V30" s="109"/>
-      <c r="W30" s="109"/>
-      <c r="X30" s="109"/>
-      <c r="Y30" s="109"/>
-      <c r="Z30" s="109"/>
-      <c r="AA30" s="109"/>
-      <c r="AB30" s="109"/>
-      <c r="AC30" s="109"/>
-      <c r="AD30" s="109"/>
-      <c r="AE30" s="109"/>
-      <c r="AF30" s="109"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+      <c r="L30" s="110"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="110"/>
+      <c r="O30" s="110"/>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="110"/>
+      <c r="R30" s="110"/>
+      <c r="S30" s="110"/>
+      <c r="T30" s="110"/>
+      <c r="U30" s="110"/>
+      <c r="V30" s="110"/>
+      <c r="W30" s="110"/>
+      <c r="X30" s="110"/>
+      <c r="Y30" s="110"/>
+      <c r="Z30" s="110"/>
+      <c r="AA30" s="110"/>
+      <c r="AB30" s="110"/>
+      <c r="AC30" s="110"/>
+      <c r="AD30" s="110"/>
+      <c r="AE30" s="110"/>
+      <c r="AF30" s="110"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="G31" s="109"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="109"/>
-      <c r="J31" s="109"/>
-      <c r="K31" s="109"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="109"/>
-      <c r="N31" s="109"/>
-      <c r="O31" s="109"/>
-      <c r="P31" s="109"/>
-      <c r="Q31" s="109"/>
-      <c r="R31" s="109"/>
-      <c r="S31" s="109"/>
-      <c r="T31" s="109"/>
-      <c r="U31" s="109"/>
-      <c r="V31" s="109"/>
-      <c r="W31" s="109"/>
-      <c r="X31" s="109"/>
-      <c r="Y31" s="109"/>
-      <c r="Z31" s="109"/>
-      <c r="AA31" s="109"/>
-      <c r="AB31" s="109"/>
-      <c r="AC31" s="109"/>
-      <c r="AD31" s="109"/>
-      <c r="AE31" s="109"/>
-      <c r="AF31" s="109"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="110"/>
+      <c r="L31" s="110"/>
+      <c r="M31" s="110"/>
+      <c r="N31" s="110"/>
+      <c r="O31" s="110"/>
+      <c r="P31" s="110"/>
+      <c r="Q31" s="110"/>
+      <c r="R31" s="110"/>
+      <c r="S31" s="110"/>
+      <c r="T31" s="110"/>
+      <c r="U31" s="110"/>
+      <c r="V31" s="110"/>
+      <c r="W31" s="110"/>
+      <c r="X31" s="110"/>
+      <c r="Y31" s="110"/>
+      <c r="Z31" s="110"/>
+      <c r="AA31" s="110"/>
+      <c r="AB31" s="110"/>
+      <c r="AC31" s="110"/>
+      <c r="AD31" s="110"/>
+      <c r="AE31" s="110"/>
+      <c r="AF31" s="110"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="166"/>
-      <c r="D32" s="166"/>
-      <c r="G32" s="109"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="109"/>
-      <c r="J32" s="109"/>
-      <c r="K32" s="109"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="109"/>
-      <c r="N32" s="109"/>
-      <c r="O32" s="109"/>
-      <c r="P32" s="109"/>
-      <c r="Q32" s="109"/>
-      <c r="R32" s="109"/>
-      <c r="S32" s="109"/>
-      <c r="T32" s="109"/>
-      <c r="U32" s="109"/>
-      <c r="V32" s="109"/>
-      <c r="W32" s="109"/>
-      <c r="X32" s="109"/>
-      <c r="Y32" s="109"/>
-      <c r="Z32" s="109"/>
-      <c r="AA32" s="109"/>
-      <c r="AB32" s="109"/>
-      <c r="AC32" s="109"/>
-      <c r="AD32" s="109"/>
-      <c r="AE32" s="109"/>
-      <c r="AF32" s="109"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="110"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="110"/>
+      <c r="P32" s="110"/>
+      <c r="Q32" s="110"/>
+      <c r="R32" s="110"/>
+      <c r="S32" s="110"/>
+      <c r="T32" s="110"/>
+      <c r="U32" s="110"/>
+      <c r="V32" s="110"/>
+      <c r="W32" s="110"/>
+      <c r="X32" s="110"/>
+      <c r="Y32" s="110"/>
+      <c r="Z32" s="110"/>
+      <c r="AA32" s="110"/>
+      <c r="AB32" s="110"/>
+      <c r="AC32" s="110"/>
+      <c r="AD32" s="110"/>
+      <c r="AE32" s="110"/>
+      <c r="AF32" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
apoyo a direccion para actualizar hitos plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
+++ b/Proyectos/2016/Planeación/Plan_proyecto_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -59,6 +59,7 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$13</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Sheet_Title" vbProcedure="false">"Plan Riesgos"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
@@ -2356,7 +2357,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Page</oddFooter>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Page</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2368,8 +2369,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4583,7 +4584,9 @@
       <c r="C15" s="22" t="n">
         <v>42463</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="22" t="n">
+        <v>42468</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A16" s="21" t="s">
@@ -4776,7 +4779,7 @@
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Page</oddFooter>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Page</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5662,8 +5665,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5904,7 +5907,7 @@
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Page</oddFooter>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Page</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6039,8 +6042,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Sans,Normal"Times New Roman,Regular"2</oddHeader>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Times New Roman,Regular"2Página</oddFooter>
+    <oddHeader>&amp;C&amp;"Sans,Regular"Times New Roman,Regular"2</oddHeader>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Times New Roman,Regular"2Página</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -10306,7 +10309,7 @@
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Page</oddFooter>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Page</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -10319,7 +10322,7 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -10551,7 +10554,7 @@
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Page</oddFooter>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Page</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -12077,7 +12080,7 @@
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Sans,Normal"Page</oddFooter>
+    <oddFooter>&amp;C&amp;"Sans,Regular"Page</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>